<commit_message>
add navigation test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases.xlsx
+++ b/Testing/Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
   <si>
     <t>Descreption</t>
   </si>
@@ -273,15 +273,6 @@
     <t>LG_20</t>
   </si>
   <si>
-    <t>Navigation bar position</t>
-  </si>
-  <si>
-    <t>Menu items display</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Home button functionality</t>
-  </si>
-  <si>
     <t>Check the " create new account " button in the log in oage</t>
   </si>
   <si>
@@ -304,6 +295,62 @@
   </si>
   <si>
     <t>verify the login page has " create new account" button for new users</t>
+  </si>
+  <si>
+    <t>check " Networking  " button functionality</t>
+  </si>
+  <si>
+    <t>check " Software " button functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check " Home " button functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check " My Profile " button functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check " Embeded Syaytems " button
+ functionality</t>
+  </si>
+  <si>
+    <t>check " Biotechnology " button 
+functionality</t>
+  </si>
+  <si>
+    <t>check " Search bar " position</t>
+  </si>
+  <si>
+    <t>check " search bar " functionality</t>
+  </si>
+  <si>
+    <t>check " ADD atricle " functionality</t>
+  </si>
+  <si>
+    <t>check " Notification " functionality</t>
+  </si>
+  <si>
+    <t>check Navigation bar position</t>
+  </si>
+  <si>
+    <t>check navigation bar items display</t>
+  </si>
+  <si>
+    <t>check Default Search results</t>
+  </si>
+  <si>
+    <t>check Patient Search Results</t>
+  </si>
+  <si>
+    <t>check  Search by auter first name</t>
+  </si>
+  <si>
+    <t>check  Search by auter last name</t>
+  </si>
+  <si>
+    <t>check  Search  by auter first and last  name</t>
+  </si>
+  <si>
+    <t>check  Search by article tittle</t>
   </si>
 </sst>
 </file>
@@ -425,13 +472,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -440,7 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,17 +768,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.88671875" style="5" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="43.21875" style="7" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" style="7" customWidth="1"/>
@@ -741,20 +788,20 @@
     <col min="11" max="11" width="15.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="10" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:28" s="4" customFormat="1" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -916,10 +963,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>68</v>
@@ -1176,10 +1223,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>68</v>
@@ -1210,16 +1257,16 @@
     </row>
     <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>68</v>
@@ -1230,7 +1277,7 @@
     </row>
     <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>18</v>
@@ -1248,34 +1295,109 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="13" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:11" s="9" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C26" s="7" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C27" s="7" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C28" s="7" t="s">
-        <v>77</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C31" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C32" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C40" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating navigation test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases.xlsx
+++ b/Testing/Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="111">
   <si>
     <t>Descreption</t>
   </si>
@@ -320,9 +320,6 @@
     <t>check " Search bar " position</t>
   </si>
   <si>
-    <t>check " search bar " functionality</t>
-  </si>
-  <si>
     <t>check " ADD atricle " functionality</t>
   </si>
   <si>
@@ -351,6 +348,39 @@
   </si>
   <si>
     <t>check  Search by article tittle</t>
+  </si>
+  <si>
+    <t>check the logo position</t>
+  </si>
+  <si>
+    <t>check response time for " home " button</t>
+  </si>
+  <si>
+    <t>check response time for "Software " button</t>
+  </si>
+  <si>
+    <t>check response time for Networking " button</t>
+  </si>
+  <si>
+    <t>check response time for for " Embeded Systems " button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check response time for " Biotechnology " button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">check response time for "Notification " button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">check response time for " Add article " button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">check response time for " My profile" button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">check response time for " Search " field </t>
+  </si>
+  <si>
+    <t>Usability</t>
   </si>
 </sst>
 </file>
@@ -768,17 +798,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB43"/>
+  <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="E34" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.88671875" style="5" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" style="7" customWidth="1"/>
     <col min="4" max="4" width="43.21875" style="7" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" style="7" customWidth="1"/>
@@ -1311,93 +1341,375 @@
       <c r="K25" s="13"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="C26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="7" t="s">
+      <c r="J29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C31" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C32" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C40" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="7" t="s">
+      <c r="J42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="7" t="s">
-        <v>96</v>
+      <c r="J43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B47" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating log in test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases.xlsx
+++ b/Testing/Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="183">
   <si>
     <t>Descreption</t>
   </si>
@@ -93,10 +93,6 @@
     <t>check logging in with a valid username and an invalid password.</t>
   </si>
   <si>
-    <t>check ‘Forgot Password’ butto
-n functionality.</t>
-  </si>
-  <si>
     <t>check the messages for invalid login.</t>
   </si>
   <si>
@@ -153,16 +149,6 @@
   </si>
   <si>
     <t>Check characters of username</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Verify if a user cannot enter the characters 
-not allowed  in the field
- (Username).</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Verify if a user cannot enter the characters 
-not allowed  in the field
- (Password).</t>
   </si>
   <si>
     <t>Verify if a user cannot enter the characters 
@@ -175,18 +161,10 @@
  (Username).</t>
   </si>
   <si>
-    <t>Verify the time taken to log in with a valid username
- and password.</t>
-  </si>
-  <si>
     <t>Verify the time taken to log in with a invalid username and password.</t>
   </si>
   <si>
     <t>check response time for log in with a invalid username and password.</t>
-  </si>
-  <si>
-    <t>Verify if the font, text color, and color coding of the
- Login page is as per the standard.</t>
   </si>
   <si>
     <t>LG_01</t>
@@ -335,9 +313,6 @@
     <t>check Default Search results</t>
   </si>
   <si>
-    <t>check Patient Search Results</t>
-  </si>
-  <si>
     <t>check  Search by auter first name</t>
   </si>
   <si>
@@ -359,9 +334,6 @@
     <t>check response time for "Software " button</t>
   </si>
   <si>
-    <t>check response time for Networking " button</t>
-  </si>
-  <si>
     <t>check response time for for " Embeded Systems " button</t>
   </si>
   <si>
@@ -381,6 +353,267 @@
   </si>
   <si>
     <t>Usability</t>
+  </si>
+  <si>
+    <t>NV_01</t>
+  </si>
+  <si>
+    <t>NV_02</t>
+  </si>
+  <si>
+    <t>NV_03</t>
+  </si>
+  <si>
+    <t>NV_04</t>
+  </si>
+  <si>
+    <t>NV_05</t>
+  </si>
+  <si>
+    <t>NV_06</t>
+  </si>
+  <si>
+    <t>NV_07</t>
+  </si>
+  <si>
+    <t>NV_08</t>
+  </si>
+  <si>
+    <t>NV_09</t>
+  </si>
+  <si>
+    <t>NV_10</t>
+  </si>
+  <si>
+    <t>NV_11</t>
+  </si>
+  <si>
+    <t>NV_12</t>
+  </si>
+  <si>
+    <t>NV_13</t>
+  </si>
+  <si>
+    <t>NV_14</t>
+  </si>
+  <si>
+    <t>NV_15</t>
+  </si>
+  <si>
+    <t>NV_16</t>
+  </si>
+  <si>
+    <t>NV_17</t>
+  </si>
+  <si>
+    <t>NV_18</t>
+  </si>
+  <si>
+    <t>NV_19</t>
+  </si>
+  <si>
+    <t>NV_20</t>
+  </si>
+  <si>
+    <t>NV_21</t>
+  </si>
+  <si>
+    <t>NV_22</t>
+  </si>
+  <si>
+    <t>NV_23</t>
+  </si>
+  <si>
+    <t>NV_24</t>
+  </si>
+  <si>
+    <t>NV_25</t>
+  </si>
+  <si>
+    <t>NV_26</t>
+  </si>
+  <si>
+    <t>Verify Navigation bar position on the screen as
+ required</t>
+  </si>
+  <si>
+    <t>Verify  the logo position on the screen as
+ required</t>
+  </si>
+  <si>
+    <t>Verify Search bar position on the screen as
+ required</t>
+  </si>
+  <si>
+    <t>Verify Menu items order and display on the screen</t>
+  </si>
+  <si>
+    <t>verify that " home " button direct the user to the 
+home page</t>
+  </si>
+  <si>
+    <t>verify that " Software " button direct the user to the Software page</t>
+  </si>
+  <si>
+    <t>verify that " Networking " button direct the user to the Networking page</t>
+  </si>
+  <si>
+    <t>verify that " Embeded Syaytems " button direct the user to the Embeded Syaytems page</t>
+  </si>
+  <si>
+    <t>verify that " Biotechnology " button direct the user to the Biotechnology page</t>
+  </si>
+  <si>
+    <t>verify that " My Profile " button direct the user to the his/her Profile page</t>
+  </si>
+  <si>
+    <t>verify that " ADD atricle " button direct the user to the ADD atricle page</t>
+  </si>
+  <si>
+    <t>verify that " Notification " button direct the user to the Notification page</t>
+  </si>
+  <si>
+    <t>verify that user can search article by the first name
+ of the auther</t>
+  </si>
+  <si>
+    <t>verify that user can search article by the last name
+ of the auther</t>
+  </si>
+  <si>
+    <t>verify that user can search article by the first and last name of the auther</t>
+  </si>
+  <si>
+    <t>verify that user can search article by the tittle of it</t>
+  </si>
+  <si>
+    <t>Verify that Search result appears under search bar and shows result list</t>
+  </si>
+  <si>
+    <t>Verify the time taken to log in with a valid username and password.</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " home " page after click the button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " "Software " page after click the button</t>
+  </si>
+  <si>
+    <t>check response time for " Networking " button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " Networking " page after click the button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " Embeded Systems " page after click the button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " Biotechnology " page after click the button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " "Notification " page after click the button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " Add article " page after click the button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to go to " My profile " page after click the button</t>
+  </si>
+  <si>
+    <t>Verify the time taken to show results " Search " page after click the button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user can log in </t>
+  </si>
+  <si>
+    <t>Verify if a user cannot login with an invalid username and a valid password.</t>
+  </si>
+  <si>
+    <t>a massage shown that 
+the password is wrong</t>
+  </si>
+  <si>
+    <t>check logging in with an  invalid username and a valid password.</t>
+  </si>
+  <si>
+    <t>a massage shown that 
+the username is wrong</t>
+  </si>
+  <si>
+    <t>a massage shown that 
+the fields are empty</t>
+  </si>
+  <si>
+    <t>a massage shown that 
+logging in is invalid</t>
+  </si>
+  <si>
+    <t>the user is directed to the 
+registration page</t>
+  </si>
+  <si>
+    <t>the user is directed to the 
+foget password page</t>
+  </si>
+  <si>
+    <t>the usercan log in with the
+ new password</t>
+  </si>
+  <si>
+    <t>clicking " enter " key is
+ working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user can't enter characters
+ more than the allowed in the username </t>
+  </si>
+  <si>
+    <t>user can't enter characters
+ more than the allowed in the password</t>
+  </si>
+  <si>
+    <t>the log in page don't allow
+SQL injections</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify if a user cannot enter the characters 
+not allowed  in the field (Username).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify if a user cannot enter the characters 
+not allowed  in the field (Password).</t>
+  </si>
+  <si>
+    <t>user can't enter characters
+ than are not allowed in the password</t>
+  </si>
+  <si>
+    <t>user can't enter characters
+ than are not allowed in the username</t>
+  </si>
+  <si>
+    <t>the password is visible
+ as asterisk or bullet signs.</t>
+  </si>
+  <si>
+    <t>user is logged out and should sign in again</t>
+  </si>
+  <si>
+    <t>the response time is as 
+required</t>
+  </si>
+  <si>
+    <t>the button appears in the page in it's position</t>
+  </si>
+  <si>
+    <t>Verify if the font, text color, and color coding of the Login page is as per the standard.</t>
+  </si>
+  <si>
+    <t>the fields  appear in the page in it's position</t>
+  </si>
+  <si>
+    <t>the  font, text color are as
+ required</t>
   </si>
 </sst>
 </file>
@@ -479,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -517,6 +750,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB52"/>
+  <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,8 +1051,9 @@
     <col min="4" max="4" width="43.21875" style="7" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="7" customWidth="1"/>
-    <col min="8" max="9" width="18" style="5" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="18" style="7" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" style="5" customWidth="1"/>
     <col min="11" max="11" width="15.77734375" style="5" customWidth="1"/>
   </cols>
@@ -828,8 +1068,8 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
@@ -856,10 +1096,10 @@
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>6</v>
@@ -887,7 +1127,7 @@
     </row>
     <row r="3" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -898,16 +1138,19 @@
       <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="H3" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="J3" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -916,418 +1159,475 @@
         <v>20</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>69</v>
+        <v>159</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>29</v>
+      <c r="H10" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="H14" s="6" t="s">
+        <v>171</v>
+      </c>
       <c r="J14" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>39</v>
+        <v>172</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>40</v>
+        <v>173</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="H18" s="6" t="s">
+        <v>177</v>
+      </c>
       <c r="J18" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>43</v>
+        <v>147</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K21" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>46</v>
+        <v>77</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>73</v>
+        <v>180</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="9" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1335,381 +1635,523 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="B26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="B27" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="B28" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="B29" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>133</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="B31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="B32" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="B33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="B34" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="B35" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="B36" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="B37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="B38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="B39" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="B40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="B41" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="B42" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="B43" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C43" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>95</v>
       </c>
+      <c r="D43" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="J43" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="B45" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>102</v>
+        <v>150</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="B46" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="B47" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="B48" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="B49" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="B50" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="B51" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B52" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish home page test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases.xlsx
+++ b/Testing/Test Cases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Learning-hub\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="7788" windowHeight="9072" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="7788" windowHeight="9072" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1190,7 +1190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1209,8 +1209,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1242,11 +1248,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1288,6 +1309,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4841,8 +4898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4860,41 +4917,41 @@
     <col min="12" max="12" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="3" customFormat="1" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16384" s="3" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="18" t="s">
         <v>169</v>
       </c>
       <c r="M1" s="1"/>
@@ -6095,20 +6152,20 @@
       <c r="ATL1" s="1"/>
     </row>
     <row r="2" spans="1:16384" s="13" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
@@ -6247,326 +6304,326 @@
       <c r="ER2" s="11"/>
     </row>
     <row r="3" spans="1:16384" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="20"/>
+      <c r="L3" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:16384" s="1" customFormat="1" ht="105.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4" t="s">
+      <c r="K4" s="20"/>
+      <c r="L4" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:16384" s="1" customFormat="1" ht="125.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4" t="s">
+      <c r="K5" s="20"/>
+      <c r="L5" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:16384" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4" t="s">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:16384" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4" t="s">
+      <c r="K7" s="20"/>
+      <c r="L7" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:16384" s="1" customFormat="1" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4" t="s">
+      <c r="K8" s="20"/>
+      <c r="L8" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:16384" s="1" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4" t="s">
+      <c r="K9" s="20"/>
+      <c r="L9" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:16384" s="1" customFormat="1" ht="127.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4" t="s">
+      <c r="K10" s="20"/>
+      <c r="L10" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:16384" s="1" customFormat="1" ht="133.19999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4" t="s">
+      <c r="K11" s="20"/>
+      <c r="L11" s="20" t="s">
         <v>171</v>
       </c>
       <c r="M11" s="5"/>
@@ -22943,900 +23000,900 @@
       <c r="XFD11" s="5"/>
     </row>
     <row r="12" spans="1:16384" s="1" customFormat="1" ht="137.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4" t="s">
+      <c r="K12" s="20"/>
+      <c r="L12" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:16384" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.4">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4" t="s">
+      <c r="K13" s="24"/>
+      <c r="L13" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:16384" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4" t="s">
+      <c r="K14" s="20"/>
+      <c r="L14" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:16384" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.4">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4" t="s">
+      <c r="K15" s="20"/>
+      <c r="L15" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:16384" s="1" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4" t="s">
+      <c r="K16" s="20"/>
+      <c r="L16" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" ht="137.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4" t="s">
+      <c r="K17" s="20"/>
+      <c r="L17" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4" t="s">
+      <c r="K18" s="24"/>
+      <c r="L18" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="1" customFormat="1" ht="147.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I19" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4" t="s">
+      <c r="K19" s="20"/>
+      <c r="L19" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="1" customFormat="1" ht="171.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4" t="s">
+      <c r="K20" s="24"/>
+      <c r="L20" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="1" customFormat="1" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4" t="s">
+      <c r="K21" s="24"/>
+      <c r="L21" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="1" customFormat="1" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4" t="s">
+      <c r="K22" s="24"/>
+      <c r="L22" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4" t="s">
+      <c r="K23" s="24"/>
+      <c r="L23" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" ht="195.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4" t="s">
+      <c r="K24" s="24"/>
+      <c r="L24" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" ht="149.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4" t="s">
+      <c r="K25" s="24"/>
+      <c r="L25" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="27" t="s">
         <v>295</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4" t="s">
+      <c r="K26" s="24"/>
+      <c r="L26" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="1" customFormat="1" ht="169.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="H27" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4" t="s">
+      <c r="K27" s="24"/>
+      <c r="L27" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4" t="s">
+      <c r="K28" s="24"/>
+      <c r="L28" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="1" customFormat="1" ht="101.4" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" ht="119.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4" t="s">
+      <c r="K30" s="20"/>
+      <c r="L30" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="1" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="H31" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4" t="s">
+      <c r="K31" s="20"/>
+      <c r="L31" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1" ht="123.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4" t="s">
+      <c r="K32" s="20"/>
+      <c r="L32" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="1" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H33" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="I33" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4" t="s">
+      <c r="K33" s="20"/>
+      <c r="L33" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="1" customFormat="1" ht="88.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="I34" s="15" t="s">
+      <c r="I34" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="J34" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4" t="s">
+      <c r="K34" s="20"/>
+      <c r="L34" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="1" customFormat="1" ht="120.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="I35" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4" t="s">
+      <c r="K35" s="20"/>
+      <c r="L35" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="1" customFormat="1" ht="106.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="H36" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="I36" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="J36" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4" t="s">
+      <c r="K36" s="20"/>
+      <c r="L36" s="20" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add name to test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases.xlsx
+++ b/Testing/Test Cases.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6000" windowWidth="7788" windowHeight="9072" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="6600" windowWidth="7788" windowHeight="9072" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="HM-Nada" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -1542,15 +1542,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1564,6 +1555,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,20 +1868,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1208" s="12" customFormat="1" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
@@ -4677,20 +4677,20 @@
       </c>
     </row>
     <row r="18" spans="1:126" s="7" customFormat="1" ht="36.6" x14ac:dyDescent="0.4">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -5116,8 +5116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6370,20 +6370,20 @@
       <c r="ATL1" s="1"/>
     </row>
     <row r="2" spans="1:16384" s="13" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
@@ -23253,39 +23253,39 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" s="35" customFormat="1" ht="168" x14ac:dyDescent="0.4">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:16384" s="32" customFormat="1" ht="168" x14ac:dyDescent="0.4">
+      <c r="A13" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31" t="s">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28" t="s">
         <v>156</v>
       </c>
     </row>
@@ -23433,39 +23433,39 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="35" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:12" s="32" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="28" t="s">
         <v>298</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31" t="s">
+      <c r="K18" s="28"/>
+      <c r="L18" s="28" t="s">
         <v>156</v>
       </c>
     </row>
@@ -23505,75 +23505,75 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="35" customFormat="1" ht="171.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="31" t="s">
+    <row r="20" spans="1:12" s="32" customFormat="1" ht="171.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="28" t="s">
         <v>300</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="J20" s="31" t="s">
+      <c r="J20" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31" t="s">
+      <c r="K20" s="28"/>
+      <c r="L20" s="28" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="35" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="31" t="s">
+    <row r="21" spans="1:12" s="32" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="J21" s="31" t="s">
+      <c r="J21" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31" t="s">
+      <c r="K21" s="28"/>
+      <c r="L21" s="28" t="s">
         <v>156</v>
       </c>
     </row>
@@ -24149,20 +24149,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1208" s="12" customFormat="1" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>

</xml_diff>

<commit_message>
add my test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases.xlsx
+++ b/Testing/Test Cases.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Learning-hub\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\Learning-hub\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6600" windowWidth="7788" windowHeight="9072" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="6600" windowWidth="7788" windowHeight="9072" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="HM-Nada" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Wafaa" sheetId="3" r:id="rId3"/>
+    <sheet name="login_module_Ragab" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="403">
   <si>
     <t>Descreption</t>
   </si>
@@ -1322,12 +1323,210 @@
   <si>
     <t>Blocked</t>
   </si>
+  <si>
+    <t>lhub_login_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify  login page with valid login cridentials </t>
+  </si>
+  <si>
+    <t>functional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1- visual studio must be installed 
+2- IIS server must be installed 
+3- google chrome or firefox web browser must be installed.
+4- user must already have registered in the website
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,   click on "Login" button
+4- type in "USERNAME" field as in test data
+5- type in "PASSWORD" field as in test data
+6- click on "Login" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+user name: test39
+password :  TesMe39$#
+email: learninghub@gmail.com
+FIRST NAME : power
+LAST NAME:  learners
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password is incorrect although there  test data is stored in the database 
+</t>
+  </si>
+  <si>
+    <t>Ragab</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>lhub_login_2</t>
+  </si>
+  <si>
+    <t>verify that Login page must contain username input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1- visual studio must be installed 
+2- IIS server must be installed 
+3- google chrome or firefox web browser must be installed.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3-   after the website is opened in firefox or google chrome web browser,   click on "Login" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "USERNAME" field exists on the login page</t>
+  </si>
+  <si>
+    <t>lhub_login_3</t>
+  </si>
+  <si>
+    <t>verify an error message to be displayed with red font “username is required” when leaving username field empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,   click on "Login" button
+4- type in "PASSWORD" field as in test data
+6- click on "Login" button
+</t>
+  </si>
+  <si>
+    <t>an error message  “username is required”  will be displayed with red font</t>
+  </si>
+  <si>
+    <t>an error message  “username is required”  is displayed with red font</t>
+  </si>
+  <si>
+    <t>lhub_login_4</t>
+  </si>
+  <si>
+    <t>verify Login page must contain password field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+ 3- after the website is opened in firefox or google chrome web browser,  click on "Login" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> " PASSWORD " field exists on the login page</t>
+  </si>
+  <si>
+    <t>lhub_login_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify an error message to be displayed with red font “password is required” when leaving the password field empty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,  click on "Login" button
+4- type in "USERNAME" field as in test data
+6- click on "Login" button
+</t>
+  </si>
+  <si>
+    <t>an error message will be displayed with red font “password is required”</t>
+  </si>
+  <si>
+    <t>an error message is displayed with red font “password is required”</t>
+  </si>
+  <si>
+    <t>lhub_login_6</t>
+  </si>
+  <si>
+    <t>after entering a valid user name and clicking on  "forget your password" button , an error message appears " password is required " , and I cannot redirect to next page which I can enter a valid emaill</t>
+  </si>
+  <si>
+    <t>verify "forget my password" functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,  click on "Login" button
+4- click on "forget your password" button
+5- enter a valid email address as provided in test data
+6- click on "send" button 
+7-  enter a valid email address as provided in test data 
+8 - enter a valid new password as provided in test data
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+user name: test39
+password :  TesMe39$#
+new password:  NewMe39$#
+email: learninghub@gmail.com
+FIRST NAME : power
+LAST NAME:  learners
+</t>
+  </si>
+  <si>
+    <t>verify Login page must contain "login" button</t>
+  </si>
+  <si>
+    <t>lhub_login_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1- visual studio must be installed 
+2- IIS server must be installed 
+3- google chrome or firefox web browser must be installed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,  click on "Login" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> " login " button exists on the login page</t>
+  </si>
+  <si>
+    <t>lhub_login_8</t>
+  </si>
+  <si>
+    <t>verify “create a new account”  link works  from login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,  click on "Login" button
+6- click on “create account”  link  
+</t>
+  </si>
+  <si>
+    <t>user will be redirected to “sign up” web page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> “sign up” web page  has appeared </t>
+  </si>
+  <si>
+    <t>user will be redirected to the home page and the "test39" is placed at the left side of the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user is redirected to “reset password “ page </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1372,8 +1571,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1402,6 +1644,16 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1466,10 +1718,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1564,8 +1818,28 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1846,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ATL27"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -5116,7 +5390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -24127,8 +24401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ATL26"/>
   <sheetViews>
-    <sheetView topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -26924,4 +27198,2735 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ATL10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" style="41" customWidth="1"/>
+    <col min="3" max="3" width="57.5546875" customWidth="1"/>
+    <col min="4" max="4" width="53.109375" customWidth="1"/>
+    <col min="5" max="5" width="76.21875" customWidth="1"/>
+    <col min="6" max="6" width="124.5546875" customWidth="1"/>
+    <col min="7" max="7" width="47.109375" customWidth="1"/>
+    <col min="8" max="8" width="49.88671875" customWidth="1"/>
+    <col min="9" max="9" width="41.44140625" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1208" s="12" customFormat="1" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11"/>
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11"/>
+      <c r="DY1" s="11"/>
+      <c r="DZ1" s="11"/>
+      <c r="EA1" s="11"/>
+      <c r="EB1" s="11"/>
+      <c r="EC1" s="11"/>
+      <c r="ED1" s="11"/>
+      <c r="EE1" s="11"/>
+      <c r="EF1" s="11"/>
+      <c r="EG1" s="11"/>
+      <c r="EH1" s="11"/>
+      <c r="EI1" s="11"/>
+      <c r="EJ1" s="11"/>
+      <c r="EK1" s="11"/>
+      <c r="EL1" s="11"/>
+      <c r="EM1" s="11"/>
+      <c r="EN1" s="11"/>
+      <c r="EO1" s="11"/>
+      <c r="EP1" s="11"/>
+      <c r="EQ1" s="11"/>
+      <c r="ER1" s="11"/>
+      <c r="ES1" s="11"/>
+      <c r="ET1" s="11"/>
+      <c r="EU1" s="11"/>
+      <c r="EV1" s="11"/>
+      <c r="EW1" s="11"/>
+      <c r="EX1" s="11"/>
+      <c r="EY1" s="11"/>
+      <c r="EZ1" s="11"/>
+      <c r="FA1" s="11"/>
+      <c r="FB1" s="11"/>
+      <c r="FC1" s="11"/>
+      <c r="FD1" s="11"/>
+      <c r="FE1" s="11"/>
+      <c r="FF1" s="11"/>
+      <c r="FG1" s="11"/>
+      <c r="FH1" s="11"/>
+      <c r="FI1" s="11"/>
+      <c r="FJ1" s="11"/>
+      <c r="FK1" s="11"/>
+      <c r="FL1" s="11"/>
+      <c r="FM1" s="11"/>
+      <c r="FN1" s="11"/>
+      <c r="FO1" s="11"/>
+      <c r="FP1" s="11"/>
+      <c r="FQ1" s="11"/>
+      <c r="FR1" s="11"/>
+      <c r="FS1" s="11"/>
+      <c r="FT1" s="11"/>
+      <c r="FU1" s="11"/>
+      <c r="FV1" s="11"/>
+      <c r="FW1" s="11"/>
+      <c r="FX1" s="11"/>
+      <c r="FY1" s="11"/>
+      <c r="FZ1" s="11"/>
+      <c r="GA1" s="11"/>
+      <c r="GB1" s="11"/>
+      <c r="GC1" s="11"/>
+      <c r="GD1" s="11"/>
+      <c r="GE1" s="11"/>
+      <c r="GF1" s="11"/>
+      <c r="GG1" s="11"/>
+      <c r="GH1" s="11"/>
+      <c r="GI1" s="11"/>
+      <c r="GJ1" s="11"/>
+      <c r="GK1" s="11"/>
+      <c r="GL1" s="11"/>
+      <c r="GM1" s="11"/>
+      <c r="GN1" s="11"/>
+      <c r="GO1" s="11"/>
+      <c r="GP1" s="11"/>
+      <c r="GQ1" s="11"/>
+      <c r="GR1" s="11"/>
+      <c r="GS1" s="11"/>
+      <c r="GT1" s="11"/>
+      <c r="GU1" s="11"/>
+      <c r="GV1" s="11"/>
+      <c r="GW1" s="11"/>
+      <c r="GX1" s="11"/>
+      <c r="GY1" s="11"/>
+      <c r="GZ1" s="11"/>
+      <c r="HA1" s="11"/>
+      <c r="HB1" s="11"/>
+      <c r="HC1" s="11"/>
+      <c r="HD1" s="11"/>
+      <c r="HE1" s="11"/>
+      <c r="HF1" s="11"/>
+      <c r="HG1" s="11"/>
+      <c r="HH1" s="11"/>
+      <c r="HI1" s="11"/>
+      <c r="HJ1" s="11"/>
+      <c r="HK1" s="11"/>
+      <c r="HL1" s="11"/>
+      <c r="HM1" s="11"/>
+      <c r="HN1" s="11"/>
+      <c r="HO1" s="11"/>
+      <c r="HP1" s="11"/>
+      <c r="HQ1" s="11"/>
+      <c r="HR1" s="11"/>
+      <c r="HS1" s="11"/>
+      <c r="HT1" s="11"/>
+      <c r="HU1" s="11"/>
+      <c r="HV1" s="11"/>
+      <c r="HW1" s="11"/>
+      <c r="HX1" s="11"/>
+      <c r="HY1" s="11"/>
+      <c r="HZ1" s="11"/>
+      <c r="IA1" s="11"/>
+      <c r="IB1" s="11"/>
+      <c r="IC1" s="11"/>
+      <c r="ID1" s="11"/>
+      <c r="IE1" s="11"/>
+      <c r="IF1" s="11"/>
+      <c r="IG1" s="11"/>
+      <c r="IH1" s="11"/>
+      <c r="II1" s="11"/>
+      <c r="IJ1" s="11"/>
+      <c r="IK1" s="11"/>
+      <c r="IL1" s="11"/>
+      <c r="IM1" s="11"/>
+      <c r="IN1" s="11"/>
+      <c r="IO1" s="11"/>
+      <c r="IP1" s="11"/>
+      <c r="IQ1" s="11"/>
+      <c r="IR1" s="11"/>
+      <c r="IS1" s="11"/>
+      <c r="IT1" s="11"/>
+      <c r="IU1" s="11"/>
+      <c r="IV1" s="11"/>
+      <c r="IW1" s="11"/>
+      <c r="IX1" s="11"/>
+      <c r="IY1" s="11"/>
+      <c r="IZ1" s="11"/>
+      <c r="JA1" s="11"/>
+      <c r="JB1" s="11"/>
+      <c r="JC1" s="11"/>
+      <c r="JD1" s="11"/>
+      <c r="JE1" s="11"/>
+      <c r="JF1" s="11"/>
+      <c r="JG1" s="11"/>
+      <c r="JH1" s="11"/>
+      <c r="JI1" s="11"/>
+      <c r="JJ1" s="11"/>
+      <c r="JK1" s="11"/>
+      <c r="JL1" s="11"/>
+      <c r="JM1" s="11"/>
+      <c r="JN1" s="11"/>
+      <c r="JO1" s="11"/>
+      <c r="JP1" s="11"/>
+      <c r="JQ1" s="11"/>
+      <c r="JR1" s="11"/>
+      <c r="JS1" s="11"/>
+      <c r="JT1" s="11"/>
+      <c r="JU1" s="11"/>
+      <c r="JV1" s="11"/>
+      <c r="JW1" s="11"/>
+      <c r="JX1" s="11"/>
+      <c r="JY1" s="11"/>
+      <c r="JZ1" s="11"/>
+      <c r="KA1" s="11"/>
+      <c r="KB1" s="11"/>
+      <c r="KC1" s="11"/>
+      <c r="KD1" s="11"/>
+      <c r="KE1" s="11"/>
+      <c r="KF1" s="11"/>
+      <c r="KG1" s="11"/>
+      <c r="KH1" s="11"/>
+      <c r="KI1" s="11"/>
+      <c r="KJ1" s="11"/>
+      <c r="KK1" s="11"/>
+      <c r="KL1" s="11"/>
+      <c r="KM1" s="11"/>
+      <c r="KN1" s="11"/>
+      <c r="KO1" s="11"/>
+      <c r="KP1" s="11"/>
+      <c r="KQ1" s="11"/>
+      <c r="KR1" s="11"/>
+      <c r="KS1" s="11"/>
+      <c r="KT1" s="11"/>
+      <c r="KU1" s="11"/>
+      <c r="KV1" s="11"/>
+      <c r="KW1" s="11"/>
+      <c r="KX1" s="11"/>
+      <c r="KY1" s="11"/>
+      <c r="KZ1" s="11"/>
+      <c r="LA1" s="11"/>
+      <c r="LB1" s="11"/>
+      <c r="LC1" s="11"/>
+      <c r="LD1" s="11"/>
+      <c r="LE1" s="11"/>
+      <c r="LF1" s="11"/>
+      <c r="LG1" s="11"/>
+      <c r="LH1" s="11"/>
+      <c r="LI1" s="11"/>
+      <c r="LJ1" s="11"/>
+      <c r="LK1" s="11"/>
+      <c r="LL1" s="11"/>
+      <c r="LM1" s="11"/>
+      <c r="LN1" s="11"/>
+      <c r="LO1" s="11"/>
+      <c r="LP1" s="11"/>
+      <c r="LQ1" s="11"/>
+      <c r="LR1" s="11"/>
+      <c r="LS1" s="11"/>
+      <c r="LT1" s="11"/>
+      <c r="LU1" s="11"/>
+      <c r="LV1" s="11"/>
+      <c r="LW1" s="11"/>
+      <c r="LX1" s="11"/>
+      <c r="LY1" s="11"/>
+      <c r="LZ1" s="11"/>
+      <c r="MA1" s="11"/>
+      <c r="MB1" s="11"/>
+      <c r="MC1" s="11"/>
+      <c r="MD1" s="11"/>
+      <c r="ME1" s="11"/>
+      <c r="MF1" s="11"/>
+      <c r="MG1" s="11"/>
+      <c r="MH1" s="11"/>
+      <c r="MI1" s="11"/>
+      <c r="MJ1" s="11"/>
+      <c r="MK1" s="11"/>
+      <c r="ML1" s="11"/>
+      <c r="MM1" s="11"/>
+      <c r="MN1" s="11"/>
+      <c r="MO1" s="11"/>
+      <c r="MP1" s="11"/>
+      <c r="MQ1" s="11"/>
+      <c r="MR1" s="11"/>
+      <c r="MS1" s="11"/>
+      <c r="MT1" s="11"/>
+      <c r="MU1" s="11"/>
+      <c r="MV1" s="11"/>
+      <c r="MW1" s="11"/>
+      <c r="MX1" s="11"/>
+      <c r="MY1" s="11"/>
+      <c r="MZ1" s="11"/>
+      <c r="NA1" s="11"/>
+      <c r="NB1" s="11"/>
+      <c r="NC1" s="11"/>
+      <c r="ND1" s="11"/>
+      <c r="NE1" s="11"/>
+      <c r="NF1" s="11"/>
+      <c r="NG1" s="11"/>
+      <c r="NH1" s="11"/>
+      <c r="NI1" s="11"/>
+      <c r="NJ1" s="11"/>
+      <c r="NK1" s="11"/>
+      <c r="NL1" s="11"/>
+      <c r="NM1" s="11"/>
+      <c r="NN1" s="11"/>
+      <c r="NO1" s="11"/>
+      <c r="NP1" s="11"/>
+      <c r="NQ1" s="11"/>
+      <c r="NR1" s="11"/>
+      <c r="NS1" s="11"/>
+      <c r="NT1" s="11"/>
+      <c r="NU1" s="11"/>
+      <c r="NV1" s="11"/>
+      <c r="NW1" s="11"/>
+      <c r="NX1" s="11"/>
+      <c r="NY1" s="11"/>
+      <c r="NZ1" s="11"/>
+      <c r="OA1" s="11"/>
+      <c r="OB1" s="11"/>
+      <c r="OC1" s="11"/>
+      <c r="OD1" s="11"/>
+      <c r="OE1" s="11"/>
+      <c r="OF1" s="11"/>
+      <c r="OG1" s="11"/>
+      <c r="OH1" s="11"/>
+      <c r="OI1" s="11"/>
+      <c r="OJ1" s="11"/>
+      <c r="OK1" s="11"/>
+      <c r="OL1" s="11"/>
+      <c r="OM1" s="11"/>
+      <c r="ON1" s="11"/>
+      <c r="OO1" s="11"/>
+      <c r="OP1" s="11"/>
+      <c r="OQ1" s="11"/>
+      <c r="OR1" s="11"/>
+      <c r="OS1" s="11"/>
+      <c r="OT1" s="11"/>
+      <c r="OU1" s="11"/>
+      <c r="OV1" s="11"/>
+      <c r="OW1" s="11"/>
+      <c r="OX1" s="11"/>
+      <c r="OY1" s="11"/>
+      <c r="OZ1" s="11"/>
+      <c r="PA1" s="11"/>
+      <c r="PB1" s="11"/>
+      <c r="PC1" s="11"/>
+      <c r="PD1" s="11"/>
+      <c r="PE1" s="11"/>
+      <c r="PF1" s="11"/>
+      <c r="PG1" s="11"/>
+      <c r="PH1" s="11"/>
+      <c r="PI1" s="11"/>
+      <c r="PJ1" s="11"/>
+      <c r="PK1" s="11"/>
+      <c r="PL1" s="11"/>
+      <c r="PM1" s="11"/>
+      <c r="PN1" s="11"/>
+      <c r="PO1" s="11"/>
+      <c r="PP1" s="11"/>
+      <c r="PQ1" s="11"/>
+      <c r="PR1" s="11"/>
+      <c r="PS1" s="11"/>
+      <c r="PT1" s="11"/>
+      <c r="PU1" s="11"/>
+      <c r="PV1" s="11"/>
+      <c r="PW1" s="11"/>
+      <c r="PX1" s="11"/>
+      <c r="PY1" s="11"/>
+      <c r="PZ1" s="11"/>
+      <c r="QA1" s="11"/>
+      <c r="QB1" s="11"/>
+      <c r="QC1" s="11"/>
+      <c r="QD1" s="11"/>
+      <c r="QE1" s="11"/>
+      <c r="QF1" s="11"/>
+      <c r="QG1" s="11"/>
+      <c r="QH1" s="11"/>
+      <c r="QI1" s="11"/>
+      <c r="QJ1" s="11"/>
+      <c r="QK1" s="11"/>
+      <c r="QL1" s="11"/>
+      <c r="QM1" s="11"/>
+      <c r="QN1" s="11"/>
+      <c r="QO1" s="11"/>
+      <c r="QP1" s="11"/>
+      <c r="QQ1" s="11"/>
+      <c r="QR1" s="11"/>
+      <c r="QS1" s="11"/>
+      <c r="QT1" s="11"/>
+      <c r="QU1" s="11"/>
+      <c r="QV1" s="11"/>
+      <c r="QW1" s="11"/>
+      <c r="QX1" s="11"/>
+      <c r="QY1" s="11"/>
+      <c r="QZ1" s="11"/>
+      <c r="RA1" s="11"/>
+      <c r="RB1" s="11"/>
+      <c r="RC1" s="11"/>
+      <c r="RD1" s="11"/>
+      <c r="RE1" s="11"/>
+      <c r="RF1" s="11"/>
+      <c r="RG1" s="11"/>
+      <c r="RH1" s="11"/>
+      <c r="RI1" s="11"/>
+      <c r="RJ1" s="11"/>
+      <c r="RK1" s="11"/>
+      <c r="RL1" s="11"/>
+      <c r="RM1" s="11"/>
+      <c r="RN1" s="11"/>
+      <c r="RO1" s="11"/>
+      <c r="RP1" s="11"/>
+      <c r="RQ1" s="11"/>
+      <c r="RR1" s="11"/>
+      <c r="RS1" s="11"/>
+      <c r="RT1" s="11"/>
+      <c r="RU1" s="11"/>
+      <c r="RV1" s="11"/>
+      <c r="RW1" s="11"/>
+      <c r="RX1" s="11"/>
+      <c r="RY1" s="11"/>
+      <c r="RZ1" s="11"/>
+      <c r="SA1" s="11"/>
+      <c r="SB1" s="11"/>
+      <c r="SC1" s="11"/>
+      <c r="SD1" s="11"/>
+      <c r="SE1" s="11"/>
+      <c r="SF1" s="11"/>
+      <c r="SG1" s="11"/>
+      <c r="SH1" s="11"/>
+      <c r="SI1" s="11"/>
+      <c r="SJ1" s="11"/>
+      <c r="SK1" s="11"/>
+      <c r="SL1" s="11"/>
+      <c r="SM1" s="11"/>
+      <c r="SN1" s="11"/>
+      <c r="SO1" s="11"/>
+      <c r="SP1" s="11"/>
+      <c r="SQ1" s="11"/>
+      <c r="SR1" s="11"/>
+      <c r="SS1" s="11"/>
+      <c r="ST1" s="11"/>
+      <c r="SU1" s="11"/>
+      <c r="SV1" s="11"/>
+      <c r="SW1" s="11"/>
+      <c r="SX1" s="11"/>
+      <c r="SY1" s="11"/>
+      <c r="SZ1" s="11"/>
+      <c r="TA1" s="11"/>
+      <c r="TB1" s="11"/>
+      <c r="TC1" s="11"/>
+      <c r="TD1" s="11"/>
+      <c r="TE1" s="11"/>
+      <c r="TF1" s="11"/>
+      <c r="TG1" s="11"/>
+      <c r="TH1" s="11"/>
+      <c r="TI1" s="11"/>
+      <c r="TJ1" s="11"/>
+      <c r="TK1" s="11"/>
+      <c r="TL1" s="11"/>
+      <c r="TM1" s="11"/>
+      <c r="TN1" s="11"/>
+      <c r="TO1" s="11"/>
+      <c r="TP1" s="11"/>
+      <c r="TQ1" s="11"/>
+      <c r="TR1" s="11"/>
+      <c r="TS1" s="11"/>
+      <c r="TT1" s="11"/>
+      <c r="TU1" s="11"/>
+      <c r="TV1" s="11"/>
+      <c r="TW1" s="11"/>
+      <c r="TX1" s="11"/>
+      <c r="TY1" s="11"/>
+      <c r="TZ1" s="11"/>
+      <c r="UA1" s="11"/>
+      <c r="UB1" s="11"/>
+      <c r="UC1" s="11"/>
+      <c r="UD1" s="11"/>
+      <c r="UE1" s="11"/>
+      <c r="UF1" s="11"/>
+      <c r="UG1" s="11"/>
+      <c r="UH1" s="11"/>
+      <c r="UI1" s="11"/>
+      <c r="UJ1" s="11"/>
+      <c r="UK1" s="11"/>
+      <c r="UL1" s="11"/>
+      <c r="UM1" s="11"/>
+      <c r="UN1" s="11"/>
+      <c r="UO1" s="11"/>
+      <c r="UP1" s="11"/>
+      <c r="UQ1" s="11"/>
+      <c r="UR1" s="11"/>
+      <c r="US1" s="11"/>
+      <c r="UT1" s="11"/>
+      <c r="UU1" s="11"/>
+      <c r="UV1" s="11"/>
+      <c r="UW1" s="11"/>
+      <c r="UX1" s="11"/>
+      <c r="UY1" s="11"/>
+      <c r="UZ1" s="11"/>
+      <c r="VA1" s="11"/>
+      <c r="VB1" s="11"/>
+      <c r="VC1" s="11"/>
+      <c r="VD1" s="11"/>
+      <c r="VE1" s="11"/>
+      <c r="VF1" s="11"/>
+      <c r="VG1" s="11"/>
+      <c r="VH1" s="11"/>
+      <c r="VI1" s="11"/>
+      <c r="VJ1" s="11"/>
+      <c r="VK1" s="11"/>
+      <c r="VL1" s="11"/>
+      <c r="VM1" s="11"/>
+      <c r="VN1" s="11"/>
+      <c r="VO1" s="11"/>
+      <c r="VP1" s="11"/>
+      <c r="VQ1" s="11"/>
+      <c r="VR1" s="11"/>
+      <c r="VS1" s="11"/>
+      <c r="VT1" s="11"/>
+      <c r="VU1" s="11"/>
+      <c r="VV1" s="11"/>
+      <c r="VW1" s="11"/>
+      <c r="VX1" s="11"/>
+      <c r="VY1" s="11"/>
+      <c r="VZ1" s="11"/>
+      <c r="WA1" s="11"/>
+      <c r="WB1" s="11"/>
+      <c r="WC1" s="11"/>
+      <c r="WD1" s="11"/>
+      <c r="WE1" s="11"/>
+      <c r="WF1" s="11"/>
+      <c r="WG1" s="11"/>
+      <c r="WH1" s="11"/>
+      <c r="WI1" s="11"/>
+      <c r="WJ1" s="11"/>
+      <c r="WK1" s="11"/>
+      <c r="WL1" s="11"/>
+      <c r="WM1" s="11"/>
+      <c r="WN1" s="11"/>
+      <c r="WO1" s="11"/>
+      <c r="WP1" s="11"/>
+      <c r="WQ1" s="11"/>
+      <c r="WR1" s="11"/>
+      <c r="WS1" s="11"/>
+      <c r="WT1" s="11"/>
+      <c r="WU1" s="11"/>
+      <c r="WV1" s="11"/>
+      <c r="WW1" s="11"/>
+      <c r="WX1" s="11"/>
+      <c r="WY1" s="11"/>
+      <c r="WZ1" s="11"/>
+      <c r="XA1" s="11"/>
+      <c r="XB1" s="11"/>
+      <c r="XC1" s="11"/>
+      <c r="XD1" s="11"/>
+      <c r="XE1" s="11"/>
+      <c r="XF1" s="11"/>
+      <c r="XG1" s="11"/>
+      <c r="XH1" s="11"/>
+      <c r="XI1" s="11"/>
+      <c r="XJ1" s="11"/>
+      <c r="XK1" s="11"/>
+      <c r="XL1" s="11"/>
+      <c r="XM1" s="11"/>
+      <c r="XN1" s="11"/>
+      <c r="XO1" s="11"/>
+      <c r="XP1" s="11"/>
+      <c r="XQ1" s="11"/>
+      <c r="XR1" s="11"/>
+      <c r="XS1" s="11"/>
+      <c r="XT1" s="11"/>
+      <c r="XU1" s="11"/>
+      <c r="XV1" s="11"/>
+      <c r="XW1" s="11"/>
+      <c r="XX1" s="11"/>
+      <c r="XY1" s="11"/>
+      <c r="XZ1" s="11"/>
+      <c r="YA1" s="11"/>
+      <c r="YB1" s="11"/>
+      <c r="YC1" s="11"/>
+      <c r="YD1" s="11"/>
+      <c r="YE1" s="11"/>
+      <c r="YF1" s="11"/>
+      <c r="YG1" s="11"/>
+      <c r="YH1" s="11"/>
+      <c r="YI1" s="11"/>
+      <c r="YJ1" s="11"/>
+      <c r="YK1" s="11"/>
+      <c r="YL1" s="11"/>
+      <c r="YM1" s="11"/>
+      <c r="YN1" s="11"/>
+      <c r="YO1" s="11"/>
+      <c r="YP1" s="11"/>
+      <c r="YQ1" s="11"/>
+      <c r="YR1" s="11"/>
+      <c r="YS1" s="11"/>
+      <c r="YT1" s="11"/>
+      <c r="YU1" s="11"/>
+      <c r="YV1" s="11"/>
+      <c r="YW1" s="11"/>
+      <c r="YX1" s="11"/>
+      <c r="YY1" s="11"/>
+      <c r="YZ1" s="11"/>
+      <c r="ZA1" s="11"/>
+      <c r="ZB1" s="11"/>
+      <c r="ZC1" s="11"/>
+      <c r="ZD1" s="11"/>
+      <c r="ZE1" s="11"/>
+      <c r="ZF1" s="11"/>
+      <c r="ZG1" s="11"/>
+      <c r="ZH1" s="11"/>
+      <c r="ZI1" s="11"/>
+      <c r="ZJ1" s="11"/>
+      <c r="ZK1" s="11"/>
+      <c r="ZL1" s="11"/>
+      <c r="ZM1" s="11"/>
+      <c r="ZN1" s="11"/>
+      <c r="ZO1" s="11"/>
+      <c r="ZP1" s="11"/>
+      <c r="ZQ1" s="11"/>
+      <c r="ZR1" s="11"/>
+      <c r="ZS1" s="11"/>
+      <c r="ZT1" s="11"/>
+      <c r="ZU1" s="11"/>
+      <c r="ZV1" s="11"/>
+      <c r="ZW1" s="11"/>
+      <c r="ZX1" s="11"/>
+      <c r="ZY1" s="11"/>
+      <c r="ZZ1" s="11"/>
+      <c r="AAA1" s="11"/>
+      <c r="AAB1" s="11"/>
+      <c r="AAC1" s="11"/>
+      <c r="AAD1" s="11"/>
+      <c r="AAE1" s="11"/>
+      <c r="AAF1" s="11"/>
+      <c r="AAG1" s="11"/>
+      <c r="AAH1" s="11"/>
+      <c r="AAI1" s="11"/>
+      <c r="AAJ1" s="11"/>
+      <c r="AAK1" s="11"/>
+      <c r="AAL1" s="11"/>
+      <c r="AAM1" s="11"/>
+      <c r="AAN1" s="11"/>
+      <c r="AAO1" s="11"/>
+      <c r="AAP1" s="11"/>
+      <c r="AAQ1" s="11"/>
+      <c r="AAR1" s="11"/>
+      <c r="AAS1" s="11"/>
+      <c r="AAT1" s="11"/>
+      <c r="AAU1" s="11"/>
+      <c r="AAV1" s="11"/>
+      <c r="AAW1" s="11"/>
+      <c r="AAX1" s="11"/>
+      <c r="AAY1" s="11"/>
+      <c r="AAZ1" s="11"/>
+      <c r="ABA1" s="11"/>
+      <c r="ABB1" s="11"/>
+      <c r="ABC1" s="11"/>
+      <c r="ABD1" s="11"/>
+      <c r="ABE1" s="11"/>
+      <c r="ABF1" s="11"/>
+      <c r="ABG1" s="11"/>
+      <c r="ABH1" s="11"/>
+      <c r="ABI1" s="11"/>
+      <c r="ABJ1" s="11"/>
+      <c r="ABK1" s="11"/>
+      <c r="ABL1" s="11"/>
+      <c r="ABM1" s="11"/>
+      <c r="ABN1" s="11"/>
+      <c r="ABO1" s="11"/>
+      <c r="ABP1" s="11"/>
+      <c r="ABQ1" s="11"/>
+      <c r="ABR1" s="11"/>
+      <c r="ABS1" s="11"/>
+      <c r="ABT1" s="11"/>
+      <c r="ABU1" s="11"/>
+      <c r="ABV1" s="11"/>
+      <c r="ABW1" s="11"/>
+      <c r="ABX1" s="11"/>
+      <c r="ABY1" s="11"/>
+      <c r="ABZ1" s="11"/>
+      <c r="ACA1" s="11"/>
+      <c r="ACB1" s="11"/>
+      <c r="ACC1" s="11"/>
+      <c r="ACD1" s="11"/>
+      <c r="ACE1" s="11"/>
+      <c r="ACF1" s="11"/>
+      <c r="ACG1" s="11"/>
+      <c r="ACH1" s="11"/>
+      <c r="ACI1" s="11"/>
+      <c r="ACJ1" s="11"/>
+      <c r="ACK1" s="11"/>
+      <c r="ACL1" s="11"/>
+      <c r="ACM1" s="11"/>
+      <c r="ACN1" s="11"/>
+      <c r="ACO1" s="11"/>
+      <c r="ACP1" s="11"/>
+      <c r="ACQ1" s="11"/>
+      <c r="ACR1" s="11"/>
+      <c r="ACS1" s="11"/>
+      <c r="ACT1" s="11"/>
+      <c r="ACU1" s="11"/>
+      <c r="ACV1" s="11"/>
+      <c r="ACW1" s="11"/>
+      <c r="ACX1" s="11"/>
+      <c r="ACY1" s="11"/>
+      <c r="ACZ1" s="11"/>
+      <c r="ADA1" s="11"/>
+      <c r="ADB1" s="11"/>
+      <c r="ADC1" s="11"/>
+      <c r="ADD1" s="11"/>
+      <c r="ADE1" s="11"/>
+      <c r="ADF1" s="11"/>
+      <c r="ADG1" s="11"/>
+      <c r="ADH1" s="11"/>
+      <c r="ADI1" s="11"/>
+      <c r="ADJ1" s="11"/>
+      <c r="ADK1" s="11"/>
+      <c r="ADL1" s="11"/>
+      <c r="ADM1" s="11"/>
+      <c r="ADN1" s="11"/>
+      <c r="ADO1" s="11"/>
+      <c r="ADP1" s="11"/>
+      <c r="ADQ1" s="11"/>
+      <c r="ADR1" s="11"/>
+      <c r="ADS1" s="11"/>
+      <c r="ADT1" s="11"/>
+      <c r="ADU1" s="11"/>
+      <c r="ADV1" s="11"/>
+      <c r="ADW1" s="11"/>
+      <c r="ADX1" s="11"/>
+      <c r="ADY1" s="11"/>
+      <c r="ADZ1" s="11"/>
+      <c r="AEA1" s="11"/>
+      <c r="AEB1" s="11"/>
+      <c r="AEC1" s="11"/>
+      <c r="AED1" s="11"/>
+      <c r="AEE1" s="11"/>
+      <c r="AEF1" s="11"/>
+      <c r="AEG1" s="11"/>
+      <c r="AEH1" s="11"/>
+      <c r="AEI1" s="11"/>
+      <c r="AEJ1" s="11"/>
+      <c r="AEK1" s="11"/>
+      <c r="AEL1" s="11"/>
+      <c r="AEM1" s="11"/>
+      <c r="AEN1" s="11"/>
+      <c r="AEO1" s="11"/>
+      <c r="AEP1" s="11"/>
+      <c r="AEQ1" s="11"/>
+      <c r="AER1" s="11"/>
+      <c r="AES1" s="11"/>
+      <c r="AET1" s="11"/>
+      <c r="AEU1" s="11"/>
+      <c r="AEV1" s="11"/>
+      <c r="AEW1" s="11"/>
+      <c r="AEX1" s="11"/>
+      <c r="AEY1" s="11"/>
+      <c r="AEZ1" s="11"/>
+      <c r="AFA1" s="11"/>
+      <c r="AFB1" s="11"/>
+      <c r="AFC1" s="11"/>
+      <c r="AFD1" s="11"/>
+      <c r="AFE1" s="11"/>
+      <c r="AFF1" s="11"/>
+      <c r="AFG1" s="11"/>
+      <c r="AFH1" s="11"/>
+      <c r="AFI1" s="11"/>
+      <c r="AFJ1" s="11"/>
+      <c r="AFK1" s="11"/>
+      <c r="AFL1" s="11"/>
+      <c r="AFM1" s="11"/>
+      <c r="AFN1" s="11"/>
+      <c r="AFO1" s="11"/>
+      <c r="AFP1" s="11"/>
+      <c r="AFQ1" s="11"/>
+      <c r="AFR1" s="11"/>
+      <c r="AFS1" s="11"/>
+      <c r="AFT1" s="11"/>
+      <c r="AFU1" s="11"/>
+      <c r="AFV1" s="11"/>
+      <c r="AFW1" s="11"/>
+      <c r="AFX1" s="11"/>
+      <c r="AFY1" s="11"/>
+      <c r="AFZ1" s="11"/>
+      <c r="AGA1" s="11"/>
+      <c r="AGB1" s="11"/>
+      <c r="AGC1" s="11"/>
+      <c r="AGD1" s="11"/>
+      <c r="AGE1" s="11"/>
+      <c r="AGF1" s="11"/>
+      <c r="AGG1" s="11"/>
+      <c r="AGH1" s="11"/>
+      <c r="AGI1" s="11"/>
+      <c r="AGJ1" s="11"/>
+      <c r="AGK1" s="11"/>
+      <c r="AGL1" s="11"/>
+      <c r="AGM1" s="11"/>
+      <c r="AGN1" s="11"/>
+      <c r="AGO1" s="11"/>
+      <c r="AGP1" s="11"/>
+      <c r="AGQ1" s="11"/>
+      <c r="AGR1" s="11"/>
+      <c r="AGS1" s="11"/>
+      <c r="AGT1" s="11"/>
+      <c r="AGU1" s="11"/>
+      <c r="AGV1" s="11"/>
+      <c r="AGW1" s="11"/>
+      <c r="AGX1" s="11"/>
+      <c r="AGY1" s="11"/>
+      <c r="AGZ1" s="11"/>
+      <c r="AHA1" s="11"/>
+      <c r="AHB1" s="11"/>
+      <c r="AHC1" s="11"/>
+      <c r="AHD1" s="11"/>
+      <c r="AHE1" s="11"/>
+      <c r="AHF1" s="11"/>
+      <c r="AHG1" s="11"/>
+      <c r="AHH1" s="11"/>
+      <c r="AHI1" s="11"/>
+      <c r="AHJ1" s="11"/>
+      <c r="AHK1" s="11"/>
+      <c r="AHL1" s="11"/>
+      <c r="AHM1" s="11"/>
+      <c r="AHN1" s="11"/>
+      <c r="AHO1" s="11"/>
+      <c r="AHP1" s="11"/>
+      <c r="AHQ1" s="11"/>
+      <c r="AHR1" s="11"/>
+      <c r="AHS1" s="11"/>
+      <c r="AHT1" s="11"/>
+      <c r="AHU1" s="11"/>
+      <c r="AHV1" s="11"/>
+      <c r="AHW1" s="11"/>
+      <c r="AHX1" s="11"/>
+      <c r="AHY1" s="11"/>
+      <c r="AHZ1" s="11"/>
+      <c r="AIA1" s="11"/>
+      <c r="AIB1" s="11"/>
+      <c r="AIC1" s="11"/>
+      <c r="AID1" s="11"/>
+      <c r="AIE1" s="11"/>
+      <c r="AIF1" s="11"/>
+      <c r="AIG1" s="11"/>
+      <c r="AIH1" s="11"/>
+      <c r="AII1" s="11"/>
+      <c r="AIJ1" s="11"/>
+      <c r="AIK1" s="11"/>
+      <c r="AIL1" s="11"/>
+      <c r="AIM1" s="11"/>
+      <c r="AIN1" s="11"/>
+      <c r="AIO1" s="11"/>
+      <c r="AIP1" s="11"/>
+      <c r="AIQ1" s="11"/>
+      <c r="AIR1" s="11"/>
+      <c r="AIS1" s="11"/>
+      <c r="AIT1" s="11"/>
+      <c r="AIU1" s="11"/>
+      <c r="AIV1" s="11"/>
+      <c r="AIW1" s="11"/>
+      <c r="AIX1" s="11"/>
+      <c r="AIY1" s="11"/>
+      <c r="AIZ1" s="11"/>
+      <c r="AJA1" s="11"/>
+      <c r="AJB1" s="11"/>
+      <c r="AJC1" s="11"/>
+      <c r="AJD1" s="11"/>
+      <c r="AJE1" s="11"/>
+      <c r="AJF1" s="11"/>
+      <c r="AJG1" s="11"/>
+      <c r="AJH1" s="11"/>
+      <c r="AJI1" s="11"/>
+      <c r="AJJ1" s="11"/>
+      <c r="AJK1" s="11"/>
+      <c r="AJL1" s="11"/>
+      <c r="AJM1" s="11"/>
+      <c r="AJN1" s="11"/>
+      <c r="AJO1" s="11"/>
+      <c r="AJP1" s="11"/>
+      <c r="AJQ1" s="11"/>
+      <c r="AJR1" s="11"/>
+      <c r="AJS1" s="11"/>
+      <c r="AJT1" s="11"/>
+      <c r="AJU1" s="11"/>
+      <c r="AJV1" s="11"/>
+      <c r="AJW1" s="11"/>
+      <c r="AJX1" s="11"/>
+      <c r="AJY1" s="11"/>
+      <c r="AJZ1" s="11"/>
+      <c r="AKA1" s="11"/>
+      <c r="AKB1" s="11"/>
+      <c r="AKC1" s="11"/>
+      <c r="AKD1" s="11"/>
+      <c r="AKE1" s="11"/>
+      <c r="AKF1" s="11"/>
+      <c r="AKG1" s="11"/>
+      <c r="AKH1" s="11"/>
+      <c r="AKI1" s="11"/>
+      <c r="AKJ1" s="11"/>
+      <c r="AKK1" s="11"/>
+      <c r="AKL1" s="11"/>
+      <c r="AKM1" s="11"/>
+      <c r="AKN1" s="11"/>
+      <c r="AKO1" s="11"/>
+      <c r="AKP1" s="11"/>
+      <c r="AKQ1" s="11"/>
+      <c r="AKR1" s="11"/>
+      <c r="AKS1" s="11"/>
+      <c r="AKT1" s="11"/>
+      <c r="AKU1" s="11"/>
+      <c r="AKV1" s="11"/>
+      <c r="AKW1" s="11"/>
+      <c r="AKX1" s="11"/>
+      <c r="AKY1" s="11"/>
+      <c r="AKZ1" s="11"/>
+      <c r="ALA1" s="11"/>
+      <c r="ALB1" s="11"/>
+      <c r="ALC1" s="11"/>
+      <c r="ALD1" s="11"/>
+      <c r="ALE1" s="11"/>
+      <c r="ALF1" s="11"/>
+      <c r="ALG1" s="11"/>
+      <c r="ALH1" s="11"/>
+      <c r="ALI1" s="11"/>
+      <c r="ALJ1" s="11"/>
+      <c r="ALK1" s="11"/>
+      <c r="ALL1" s="11"/>
+      <c r="ALM1" s="11"/>
+      <c r="ALN1" s="11"/>
+      <c r="ALO1" s="11"/>
+      <c r="ALP1" s="11"/>
+      <c r="ALQ1" s="11"/>
+      <c r="ALR1" s="11"/>
+      <c r="ALS1" s="11"/>
+      <c r="ALT1" s="11"/>
+      <c r="ALU1" s="11"/>
+      <c r="ALV1" s="11"/>
+      <c r="ALW1" s="11"/>
+      <c r="ALX1" s="11"/>
+      <c r="ALY1" s="11"/>
+      <c r="ALZ1" s="11"/>
+      <c r="AMA1" s="11"/>
+      <c r="AMB1" s="11"/>
+      <c r="AMC1" s="11"/>
+      <c r="AMD1" s="11"/>
+      <c r="AME1" s="11"/>
+      <c r="AMF1" s="11"/>
+      <c r="AMG1" s="11"/>
+      <c r="AMH1" s="11"/>
+      <c r="AMI1" s="11"/>
+      <c r="AMJ1" s="11"/>
+      <c r="AMK1" s="11"/>
+      <c r="AML1" s="11"/>
+      <c r="AMM1" s="11"/>
+      <c r="AMN1" s="11"/>
+      <c r="AMO1" s="11"/>
+      <c r="AMP1" s="11"/>
+      <c r="AMQ1" s="11"/>
+      <c r="AMR1" s="11"/>
+      <c r="AMS1" s="11"/>
+      <c r="AMT1" s="11"/>
+      <c r="AMU1" s="11"/>
+      <c r="AMV1" s="11"/>
+      <c r="AMW1" s="11"/>
+      <c r="AMX1" s="11"/>
+      <c r="AMY1" s="11"/>
+      <c r="AMZ1" s="11"/>
+      <c r="ANA1" s="11"/>
+      <c r="ANB1" s="11"/>
+      <c r="ANC1" s="11"/>
+      <c r="AND1" s="11"/>
+      <c r="ANE1" s="11"/>
+      <c r="ANF1" s="11"/>
+      <c r="ANG1" s="11"/>
+      <c r="ANH1" s="11"/>
+      <c r="ANI1" s="11"/>
+      <c r="ANJ1" s="11"/>
+      <c r="ANK1" s="11"/>
+      <c r="ANL1" s="11"/>
+      <c r="ANM1" s="11"/>
+      <c r="ANN1" s="11"/>
+      <c r="ANO1" s="11"/>
+      <c r="ANP1" s="11"/>
+      <c r="ANQ1" s="11"/>
+      <c r="ANR1" s="11"/>
+      <c r="ANS1" s="11"/>
+      <c r="ANT1" s="11"/>
+      <c r="ANU1" s="11"/>
+      <c r="ANV1" s="11"/>
+      <c r="ANW1" s="11"/>
+      <c r="ANX1" s="11"/>
+      <c r="ANY1" s="11"/>
+      <c r="ANZ1" s="11"/>
+      <c r="AOA1" s="11"/>
+      <c r="AOB1" s="11"/>
+      <c r="AOC1" s="11"/>
+      <c r="AOD1" s="11"/>
+      <c r="AOE1" s="11"/>
+      <c r="AOF1" s="11"/>
+      <c r="AOG1" s="11"/>
+      <c r="AOH1" s="11"/>
+      <c r="AOI1" s="11"/>
+      <c r="AOJ1" s="11"/>
+      <c r="AOK1" s="11"/>
+      <c r="AOL1" s="11"/>
+      <c r="AOM1" s="11"/>
+      <c r="AON1" s="11"/>
+      <c r="AOO1" s="11"/>
+      <c r="AOP1" s="11"/>
+      <c r="AOQ1" s="11"/>
+      <c r="AOR1" s="11"/>
+      <c r="AOS1" s="11"/>
+      <c r="AOT1" s="11"/>
+      <c r="AOU1" s="11"/>
+      <c r="AOV1" s="11"/>
+      <c r="AOW1" s="11"/>
+      <c r="AOX1" s="11"/>
+      <c r="AOY1" s="11"/>
+      <c r="AOZ1" s="11"/>
+      <c r="APA1" s="11"/>
+      <c r="APB1" s="11"/>
+      <c r="APC1" s="11"/>
+      <c r="APD1" s="11"/>
+      <c r="APE1" s="11"/>
+      <c r="APF1" s="11"/>
+      <c r="APG1" s="11"/>
+      <c r="APH1" s="11"/>
+      <c r="API1" s="11"/>
+      <c r="APJ1" s="11"/>
+      <c r="APK1" s="11"/>
+      <c r="APL1" s="11"/>
+      <c r="APM1" s="11"/>
+      <c r="APN1" s="11"/>
+      <c r="APO1" s="11"/>
+      <c r="APP1" s="11"/>
+      <c r="APQ1" s="11"/>
+      <c r="APR1" s="11"/>
+      <c r="APS1" s="11"/>
+      <c r="APT1" s="11"/>
+      <c r="APU1" s="11"/>
+      <c r="APV1" s="11"/>
+      <c r="APW1" s="11"/>
+      <c r="APX1" s="11"/>
+      <c r="APY1" s="11"/>
+      <c r="APZ1" s="11"/>
+      <c r="AQA1" s="11"/>
+      <c r="AQB1" s="11"/>
+      <c r="AQC1" s="11"/>
+      <c r="AQD1" s="11"/>
+      <c r="AQE1" s="11"/>
+      <c r="AQF1" s="11"/>
+      <c r="AQG1" s="11"/>
+      <c r="AQH1" s="11"/>
+      <c r="AQI1" s="11"/>
+      <c r="AQJ1" s="11"/>
+      <c r="AQK1" s="11"/>
+      <c r="AQL1" s="11"/>
+      <c r="AQM1" s="11"/>
+      <c r="AQN1" s="11"/>
+      <c r="AQO1" s="11"/>
+      <c r="AQP1" s="11"/>
+      <c r="AQQ1" s="11"/>
+      <c r="AQR1" s="11"/>
+      <c r="AQS1" s="11"/>
+      <c r="AQT1" s="11"/>
+      <c r="AQU1" s="11"/>
+      <c r="AQV1" s="11"/>
+      <c r="AQW1" s="11"/>
+      <c r="AQX1" s="11"/>
+      <c r="AQY1" s="11"/>
+      <c r="AQZ1" s="11"/>
+      <c r="ARA1" s="11"/>
+      <c r="ARB1" s="11"/>
+      <c r="ARC1" s="11"/>
+      <c r="ARD1" s="11"/>
+      <c r="ARE1" s="11"/>
+      <c r="ARF1" s="11"/>
+      <c r="ARG1" s="11"/>
+      <c r="ARH1" s="11"/>
+      <c r="ARI1" s="11"/>
+      <c r="ARJ1" s="11"/>
+      <c r="ARK1" s="11"/>
+      <c r="ARL1" s="11"/>
+      <c r="ARM1" s="11"/>
+      <c r="ARN1" s="11"/>
+      <c r="ARO1" s="11"/>
+      <c r="ARP1" s="11"/>
+      <c r="ARQ1" s="11"/>
+      <c r="ARR1" s="11"/>
+      <c r="ARS1" s="11"/>
+      <c r="ART1" s="11"/>
+      <c r="ARU1" s="11"/>
+      <c r="ARV1" s="11"/>
+      <c r="ARW1" s="11"/>
+      <c r="ARX1" s="11"/>
+      <c r="ARY1" s="11"/>
+      <c r="ARZ1" s="11"/>
+      <c r="ASA1" s="11"/>
+      <c r="ASB1" s="11"/>
+      <c r="ASC1" s="11"/>
+      <c r="ASD1" s="11"/>
+      <c r="ASE1" s="11"/>
+      <c r="ASF1" s="11"/>
+      <c r="ASG1" s="11"/>
+      <c r="ASH1" s="11"/>
+      <c r="ASI1" s="11"/>
+      <c r="ASJ1" s="11"/>
+      <c r="ASK1" s="11"/>
+      <c r="ASL1" s="11"/>
+      <c r="ASM1" s="11"/>
+      <c r="ASN1" s="11"/>
+      <c r="ASO1" s="11"/>
+      <c r="ASP1" s="11"/>
+      <c r="ASQ1" s="11"/>
+      <c r="ASR1" s="11"/>
+      <c r="ASS1" s="11"/>
+      <c r="AST1" s="11"/>
+      <c r="ASU1" s="11"/>
+      <c r="ASV1" s="11"/>
+      <c r="ASW1" s="11"/>
+      <c r="ASX1" s="11"/>
+      <c r="ASY1" s="11"/>
+      <c r="ASZ1" s="11"/>
+      <c r="ATA1" s="11"/>
+      <c r="ATB1" s="11"/>
+      <c r="ATC1" s="11"/>
+      <c r="ATD1" s="11"/>
+      <c r="ATE1" s="11"/>
+      <c r="ATF1" s="11"/>
+      <c r="ATG1" s="11"/>
+      <c r="ATH1" s="11"/>
+      <c r="ATI1" s="11"/>
+      <c r="ATJ1" s="11"/>
+      <c r="ATK1" s="11"/>
+      <c r="ATL1" s="11"/>
+    </row>
+    <row r="2" spans="1:1208" s="3" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+      <c r="BQ2" s="1"/>
+      <c r="BR2" s="1"/>
+      <c r="BS2" s="1"/>
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+      <c r="BV2" s="1"/>
+      <c r="BW2" s="1"/>
+      <c r="BX2" s="1"/>
+      <c r="BY2" s="1"/>
+      <c r="BZ2" s="1"/>
+      <c r="CA2" s="1"/>
+      <c r="CB2" s="1"/>
+      <c r="CC2" s="1"/>
+      <c r="CD2" s="1"/>
+      <c r="CE2" s="1"/>
+      <c r="CF2" s="1"/>
+      <c r="CG2" s="1"/>
+      <c r="CH2" s="1"/>
+      <c r="CI2" s="1"/>
+      <c r="CJ2" s="1"/>
+      <c r="CK2" s="1"/>
+      <c r="CL2" s="1"/>
+      <c r="CM2" s="1"/>
+      <c r="CN2" s="1"/>
+      <c r="CO2" s="1"/>
+      <c r="CP2" s="1"/>
+      <c r="CQ2" s="1"/>
+      <c r="CR2" s="1"/>
+      <c r="CS2" s="1"/>
+      <c r="CT2" s="1"/>
+      <c r="CU2" s="1"/>
+      <c r="CV2" s="1"/>
+      <c r="CW2" s="1"/>
+      <c r="CX2" s="1"/>
+      <c r="CY2" s="1"/>
+      <c r="CZ2" s="1"/>
+      <c r="DA2" s="1"/>
+      <c r="DB2" s="1"/>
+      <c r="DC2" s="1"/>
+      <c r="DD2" s="1"/>
+      <c r="DE2" s="1"/>
+      <c r="DF2" s="1"/>
+      <c r="DG2" s="1"/>
+      <c r="DH2" s="1"/>
+      <c r="DI2" s="1"/>
+      <c r="DJ2" s="1"/>
+      <c r="DK2" s="1"/>
+      <c r="DL2" s="1"/>
+      <c r="DM2" s="1"/>
+      <c r="DN2" s="1"/>
+      <c r="DO2" s="1"/>
+      <c r="DP2" s="1"/>
+      <c r="DQ2" s="1"/>
+      <c r="DR2" s="1"/>
+      <c r="DS2" s="1"/>
+      <c r="DT2" s="1"/>
+      <c r="DU2" s="1"/>
+      <c r="DV2" s="1"/>
+      <c r="DW2" s="1"/>
+      <c r="DX2" s="1"/>
+      <c r="DY2" s="1"/>
+      <c r="DZ2" s="1"/>
+      <c r="EA2" s="1"/>
+      <c r="EB2" s="1"/>
+      <c r="EC2" s="1"/>
+      <c r="ED2" s="1"/>
+      <c r="EE2" s="1"/>
+      <c r="EF2" s="1"/>
+      <c r="EG2" s="1"/>
+      <c r="EH2" s="1"/>
+      <c r="EI2" s="1"/>
+      <c r="EJ2" s="1"/>
+      <c r="EK2" s="1"/>
+      <c r="EL2" s="1"/>
+      <c r="EM2" s="1"/>
+      <c r="EN2" s="1"/>
+      <c r="EO2" s="1"/>
+      <c r="EP2" s="1"/>
+      <c r="EQ2" s="1"/>
+      <c r="ER2" s="1"/>
+      <c r="ES2" s="1"/>
+      <c r="ET2" s="1"/>
+      <c r="EU2" s="1"/>
+      <c r="EV2" s="1"/>
+      <c r="EW2" s="1"/>
+      <c r="EX2" s="1"/>
+      <c r="EY2" s="1"/>
+      <c r="EZ2" s="1"/>
+      <c r="FA2" s="1"/>
+      <c r="FB2" s="1"/>
+      <c r="FC2" s="1"/>
+      <c r="FD2" s="1"/>
+      <c r="FE2" s="1"/>
+      <c r="FF2" s="1"/>
+      <c r="FG2" s="1"/>
+      <c r="FH2" s="1"/>
+      <c r="FI2" s="1"/>
+      <c r="FJ2" s="1"/>
+      <c r="FK2" s="1"/>
+      <c r="FL2" s="1"/>
+      <c r="FM2" s="1"/>
+      <c r="FN2" s="1"/>
+      <c r="FO2" s="1"/>
+      <c r="FP2" s="1"/>
+      <c r="FQ2" s="1"/>
+      <c r="FR2" s="1"/>
+      <c r="FS2" s="1"/>
+      <c r="FT2" s="1"/>
+      <c r="FU2" s="1"/>
+      <c r="FV2" s="1"/>
+      <c r="FW2" s="1"/>
+      <c r="FX2" s="1"/>
+      <c r="FY2" s="1"/>
+      <c r="FZ2" s="1"/>
+      <c r="GA2" s="1"/>
+      <c r="GB2" s="1"/>
+      <c r="GC2" s="1"/>
+      <c r="GD2" s="1"/>
+      <c r="GE2" s="1"/>
+      <c r="GF2" s="1"/>
+      <c r="GG2" s="1"/>
+      <c r="GH2" s="1"/>
+      <c r="GI2" s="1"/>
+      <c r="GJ2" s="1"/>
+      <c r="GK2" s="1"/>
+      <c r="GL2" s="1"/>
+      <c r="GM2" s="1"/>
+      <c r="GN2" s="1"/>
+      <c r="GO2" s="1"/>
+      <c r="GP2" s="1"/>
+      <c r="GQ2" s="1"/>
+      <c r="GR2" s="1"/>
+      <c r="GS2" s="1"/>
+      <c r="GT2" s="1"/>
+      <c r="GU2" s="1"/>
+      <c r="GV2" s="1"/>
+      <c r="GW2" s="1"/>
+      <c r="GX2" s="1"/>
+      <c r="GY2" s="1"/>
+      <c r="GZ2" s="1"/>
+      <c r="HA2" s="1"/>
+      <c r="HB2" s="1"/>
+      <c r="HC2" s="1"/>
+      <c r="HD2" s="1"/>
+      <c r="HE2" s="1"/>
+      <c r="HF2" s="1"/>
+      <c r="HG2" s="1"/>
+      <c r="HH2" s="1"/>
+      <c r="HI2" s="1"/>
+      <c r="HJ2" s="1"/>
+      <c r="HK2" s="1"/>
+      <c r="HL2" s="1"/>
+      <c r="HM2" s="1"/>
+      <c r="HN2" s="1"/>
+      <c r="HO2" s="1"/>
+      <c r="HP2" s="1"/>
+      <c r="HQ2" s="1"/>
+      <c r="HR2" s="1"/>
+      <c r="HS2" s="1"/>
+      <c r="HT2" s="1"/>
+      <c r="HU2" s="1"/>
+      <c r="HV2" s="1"/>
+      <c r="HW2" s="1"/>
+      <c r="HX2" s="1"/>
+      <c r="HY2" s="1"/>
+      <c r="HZ2" s="1"/>
+      <c r="IA2" s="1"/>
+      <c r="IB2" s="1"/>
+      <c r="IC2" s="1"/>
+      <c r="ID2" s="1"/>
+      <c r="IE2" s="1"/>
+      <c r="IF2" s="1"/>
+      <c r="IG2" s="1"/>
+      <c r="IH2" s="1"/>
+      <c r="II2" s="1"/>
+      <c r="IJ2" s="1"/>
+      <c r="IK2" s="1"/>
+      <c r="IL2" s="1"/>
+      <c r="IM2" s="1"/>
+      <c r="IN2" s="1"/>
+      <c r="IO2" s="1"/>
+      <c r="IP2" s="1"/>
+      <c r="IQ2" s="1"/>
+      <c r="IR2" s="1"/>
+      <c r="IS2" s="1"/>
+      <c r="IT2" s="1"/>
+      <c r="IU2" s="1"/>
+      <c r="IV2" s="1"/>
+      <c r="IW2" s="1"/>
+      <c r="IX2" s="1"/>
+      <c r="IY2" s="1"/>
+      <c r="IZ2" s="1"/>
+      <c r="JA2" s="1"/>
+      <c r="JB2" s="1"/>
+      <c r="JC2" s="1"/>
+      <c r="JD2" s="1"/>
+      <c r="JE2" s="1"/>
+      <c r="JF2" s="1"/>
+      <c r="JG2" s="1"/>
+      <c r="JH2" s="1"/>
+      <c r="JI2" s="1"/>
+      <c r="JJ2" s="1"/>
+      <c r="JK2" s="1"/>
+      <c r="JL2" s="1"/>
+      <c r="JM2" s="1"/>
+      <c r="JN2" s="1"/>
+      <c r="JO2" s="1"/>
+      <c r="JP2" s="1"/>
+      <c r="JQ2" s="1"/>
+      <c r="JR2" s="1"/>
+      <c r="JS2" s="1"/>
+      <c r="JT2" s="1"/>
+      <c r="JU2" s="1"/>
+      <c r="JV2" s="1"/>
+      <c r="JW2" s="1"/>
+      <c r="JX2" s="1"/>
+      <c r="JY2" s="1"/>
+      <c r="JZ2" s="1"/>
+      <c r="KA2" s="1"/>
+      <c r="KB2" s="1"/>
+      <c r="KC2" s="1"/>
+      <c r="KD2" s="1"/>
+      <c r="KE2" s="1"/>
+      <c r="KF2" s="1"/>
+      <c r="KG2" s="1"/>
+      <c r="KH2" s="1"/>
+      <c r="KI2" s="1"/>
+      <c r="KJ2" s="1"/>
+      <c r="KK2" s="1"/>
+      <c r="KL2" s="1"/>
+      <c r="KM2" s="1"/>
+      <c r="KN2" s="1"/>
+      <c r="KO2" s="1"/>
+      <c r="KP2" s="1"/>
+      <c r="KQ2" s="1"/>
+      <c r="KR2" s="1"/>
+      <c r="KS2" s="1"/>
+      <c r="KT2" s="1"/>
+      <c r="KU2" s="1"/>
+      <c r="KV2" s="1"/>
+      <c r="KW2" s="1"/>
+      <c r="KX2" s="1"/>
+      <c r="KY2" s="1"/>
+      <c r="KZ2" s="1"/>
+      <c r="LA2" s="1"/>
+      <c r="LB2" s="1"/>
+      <c r="LC2" s="1"/>
+      <c r="LD2" s="1"/>
+      <c r="LE2" s="1"/>
+      <c r="LF2" s="1"/>
+      <c r="LG2" s="1"/>
+      <c r="LH2" s="1"/>
+      <c r="LI2" s="1"/>
+      <c r="LJ2" s="1"/>
+      <c r="LK2" s="1"/>
+      <c r="LL2" s="1"/>
+      <c r="LM2" s="1"/>
+      <c r="LN2" s="1"/>
+      <c r="LO2" s="1"/>
+      <c r="LP2" s="1"/>
+      <c r="LQ2" s="1"/>
+      <c r="LR2" s="1"/>
+      <c r="LS2" s="1"/>
+      <c r="LT2" s="1"/>
+      <c r="LU2" s="1"/>
+      <c r="LV2" s="1"/>
+      <c r="LW2" s="1"/>
+      <c r="LX2" s="1"/>
+      <c r="LY2" s="1"/>
+      <c r="LZ2" s="1"/>
+      <c r="MA2" s="1"/>
+      <c r="MB2" s="1"/>
+      <c r="MC2" s="1"/>
+      <c r="MD2" s="1"/>
+      <c r="ME2" s="1"/>
+      <c r="MF2" s="1"/>
+      <c r="MG2" s="1"/>
+      <c r="MH2" s="1"/>
+      <c r="MI2" s="1"/>
+      <c r="MJ2" s="1"/>
+      <c r="MK2" s="1"/>
+      <c r="ML2" s="1"/>
+      <c r="MM2" s="1"/>
+      <c r="MN2" s="1"/>
+      <c r="MO2" s="1"/>
+      <c r="MP2" s="1"/>
+      <c r="MQ2" s="1"/>
+      <c r="MR2" s="1"/>
+      <c r="MS2" s="1"/>
+      <c r="MT2" s="1"/>
+      <c r="MU2" s="1"/>
+      <c r="MV2" s="1"/>
+      <c r="MW2" s="1"/>
+      <c r="MX2" s="1"/>
+      <c r="MY2" s="1"/>
+      <c r="MZ2" s="1"/>
+      <c r="NA2" s="1"/>
+      <c r="NB2" s="1"/>
+      <c r="NC2" s="1"/>
+      <c r="ND2" s="1"/>
+      <c r="NE2" s="1"/>
+      <c r="NF2" s="1"/>
+      <c r="NG2" s="1"/>
+      <c r="NH2" s="1"/>
+      <c r="NI2" s="1"/>
+      <c r="NJ2" s="1"/>
+      <c r="NK2" s="1"/>
+      <c r="NL2" s="1"/>
+      <c r="NM2" s="1"/>
+      <c r="NN2" s="1"/>
+      <c r="NO2" s="1"/>
+      <c r="NP2" s="1"/>
+      <c r="NQ2" s="1"/>
+      <c r="NR2" s="1"/>
+      <c r="NS2" s="1"/>
+      <c r="NT2" s="1"/>
+      <c r="NU2" s="1"/>
+      <c r="NV2" s="1"/>
+      <c r="NW2" s="1"/>
+      <c r="NX2" s="1"/>
+      <c r="NY2" s="1"/>
+      <c r="NZ2" s="1"/>
+      <c r="OA2" s="1"/>
+      <c r="OB2" s="1"/>
+      <c r="OC2" s="1"/>
+      <c r="OD2" s="1"/>
+      <c r="OE2" s="1"/>
+      <c r="OF2" s="1"/>
+      <c r="OG2" s="1"/>
+      <c r="OH2" s="1"/>
+      <c r="OI2" s="1"/>
+      <c r="OJ2" s="1"/>
+      <c r="OK2" s="1"/>
+      <c r="OL2" s="1"/>
+      <c r="OM2" s="1"/>
+      <c r="ON2" s="1"/>
+      <c r="OO2" s="1"/>
+      <c r="OP2" s="1"/>
+      <c r="OQ2" s="1"/>
+      <c r="OR2" s="1"/>
+      <c r="OS2" s="1"/>
+      <c r="OT2" s="1"/>
+      <c r="OU2" s="1"/>
+      <c r="OV2" s="1"/>
+      <c r="OW2" s="1"/>
+      <c r="OX2" s="1"/>
+      <c r="OY2" s="1"/>
+      <c r="OZ2" s="1"/>
+      <c r="PA2" s="1"/>
+      <c r="PB2" s="1"/>
+      <c r="PC2" s="1"/>
+      <c r="PD2" s="1"/>
+      <c r="PE2" s="1"/>
+      <c r="PF2" s="1"/>
+      <c r="PG2" s="1"/>
+      <c r="PH2" s="1"/>
+      <c r="PI2" s="1"/>
+      <c r="PJ2" s="1"/>
+      <c r="PK2" s="1"/>
+      <c r="PL2" s="1"/>
+      <c r="PM2" s="1"/>
+      <c r="PN2" s="1"/>
+      <c r="PO2" s="1"/>
+      <c r="PP2" s="1"/>
+      <c r="PQ2" s="1"/>
+      <c r="PR2" s="1"/>
+      <c r="PS2" s="1"/>
+      <c r="PT2" s="1"/>
+      <c r="PU2" s="1"/>
+      <c r="PV2" s="1"/>
+      <c r="PW2" s="1"/>
+      <c r="PX2" s="1"/>
+      <c r="PY2" s="1"/>
+      <c r="PZ2" s="1"/>
+      <c r="QA2" s="1"/>
+      <c r="QB2" s="1"/>
+      <c r="QC2" s="1"/>
+      <c r="QD2" s="1"/>
+      <c r="QE2" s="1"/>
+      <c r="QF2" s="1"/>
+      <c r="QG2" s="1"/>
+      <c r="QH2" s="1"/>
+      <c r="QI2" s="1"/>
+      <c r="QJ2" s="1"/>
+      <c r="QK2" s="1"/>
+      <c r="QL2" s="1"/>
+      <c r="QM2" s="1"/>
+      <c r="QN2" s="1"/>
+      <c r="QO2" s="1"/>
+      <c r="QP2" s="1"/>
+      <c r="QQ2" s="1"/>
+      <c r="QR2" s="1"/>
+      <c r="QS2" s="1"/>
+      <c r="QT2" s="1"/>
+      <c r="QU2" s="1"/>
+      <c r="QV2" s="1"/>
+      <c r="QW2" s="1"/>
+      <c r="QX2" s="1"/>
+      <c r="QY2" s="1"/>
+      <c r="QZ2" s="1"/>
+      <c r="RA2" s="1"/>
+      <c r="RB2" s="1"/>
+      <c r="RC2" s="1"/>
+      <c r="RD2" s="1"/>
+      <c r="RE2" s="1"/>
+      <c r="RF2" s="1"/>
+      <c r="RG2" s="1"/>
+      <c r="RH2" s="1"/>
+      <c r="RI2" s="1"/>
+      <c r="RJ2" s="1"/>
+      <c r="RK2" s="1"/>
+      <c r="RL2" s="1"/>
+      <c r="RM2" s="1"/>
+      <c r="RN2" s="1"/>
+      <c r="RO2" s="1"/>
+      <c r="RP2" s="1"/>
+      <c r="RQ2" s="1"/>
+      <c r="RR2" s="1"/>
+      <c r="RS2" s="1"/>
+      <c r="RT2" s="1"/>
+      <c r="RU2" s="1"/>
+      <c r="RV2" s="1"/>
+      <c r="RW2" s="1"/>
+      <c r="RX2" s="1"/>
+      <c r="RY2" s="1"/>
+      <c r="RZ2" s="1"/>
+      <c r="SA2" s="1"/>
+      <c r="SB2" s="1"/>
+      <c r="SC2" s="1"/>
+      <c r="SD2" s="1"/>
+      <c r="SE2" s="1"/>
+      <c r="SF2" s="1"/>
+      <c r="SG2" s="1"/>
+      <c r="SH2" s="1"/>
+      <c r="SI2" s="1"/>
+      <c r="SJ2" s="1"/>
+      <c r="SK2" s="1"/>
+      <c r="SL2" s="1"/>
+      <c r="SM2" s="1"/>
+      <c r="SN2" s="1"/>
+      <c r="SO2" s="1"/>
+      <c r="SP2" s="1"/>
+      <c r="SQ2" s="1"/>
+      <c r="SR2" s="1"/>
+      <c r="SS2" s="1"/>
+      <c r="ST2" s="1"/>
+      <c r="SU2" s="1"/>
+      <c r="SV2" s="1"/>
+      <c r="SW2" s="1"/>
+      <c r="SX2" s="1"/>
+      <c r="SY2" s="1"/>
+      <c r="SZ2" s="1"/>
+      <c r="TA2" s="1"/>
+      <c r="TB2" s="1"/>
+      <c r="TC2" s="1"/>
+      <c r="TD2" s="1"/>
+      <c r="TE2" s="1"/>
+      <c r="TF2" s="1"/>
+      <c r="TG2" s="1"/>
+      <c r="TH2" s="1"/>
+      <c r="TI2" s="1"/>
+      <c r="TJ2" s="1"/>
+      <c r="TK2" s="1"/>
+      <c r="TL2" s="1"/>
+      <c r="TM2" s="1"/>
+      <c r="TN2" s="1"/>
+      <c r="TO2" s="1"/>
+      <c r="TP2" s="1"/>
+      <c r="TQ2" s="1"/>
+      <c r="TR2" s="1"/>
+      <c r="TS2" s="1"/>
+      <c r="TT2" s="1"/>
+      <c r="TU2" s="1"/>
+      <c r="TV2" s="1"/>
+      <c r="TW2" s="1"/>
+      <c r="TX2" s="1"/>
+      <c r="TY2" s="1"/>
+      <c r="TZ2" s="1"/>
+      <c r="UA2" s="1"/>
+      <c r="UB2" s="1"/>
+      <c r="UC2" s="1"/>
+      <c r="UD2" s="1"/>
+      <c r="UE2" s="1"/>
+      <c r="UF2" s="1"/>
+      <c r="UG2" s="1"/>
+      <c r="UH2" s="1"/>
+      <c r="UI2" s="1"/>
+      <c r="UJ2" s="1"/>
+      <c r="UK2" s="1"/>
+      <c r="UL2" s="1"/>
+      <c r="UM2" s="1"/>
+      <c r="UN2" s="1"/>
+      <c r="UO2" s="1"/>
+      <c r="UP2" s="1"/>
+      <c r="UQ2" s="1"/>
+      <c r="UR2" s="1"/>
+      <c r="US2" s="1"/>
+      <c r="UT2" s="1"/>
+      <c r="UU2" s="1"/>
+      <c r="UV2" s="1"/>
+      <c r="UW2" s="1"/>
+      <c r="UX2" s="1"/>
+      <c r="UY2" s="1"/>
+      <c r="UZ2" s="1"/>
+      <c r="VA2" s="1"/>
+      <c r="VB2" s="1"/>
+      <c r="VC2" s="1"/>
+      <c r="VD2" s="1"/>
+      <c r="VE2" s="1"/>
+      <c r="VF2" s="1"/>
+      <c r="VG2" s="1"/>
+      <c r="VH2" s="1"/>
+      <c r="VI2" s="1"/>
+      <c r="VJ2" s="1"/>
+      <c r="VK2" s="1"/>
+      <c r="VL2" s="1"/>
+      <c r="VM2" s="1"/>
+      <c r="VN2" s="1"/>
+      <c r="VO2" s="1"/>
+      <c r="VP2" s="1"/>
+      <c r="VQ2" s="1"/>
+      <c r="VR2" s="1"/>
+      <c r="VS2" s="1"/>
+      <c r="VT2" s="1"/>
+      <c r="VU2" s="1"/>
+      <c r="VV2" s="1"/>
+      <c r="VW2" s="1"/>
+      <c r="VX2" s="1"/>
+      <c r="VY2" s="1"/>
+      <c r="VZ2" s="1"/>
+      <c r="WA2" s="1"/>
+      <c r="WB2" s="1"/>
+      <c r="WC2" s="1"/>
+      <c r="WD2" s="1"/>
+      <c r="WE2" s="1"/>
+      <c r="WF2" s="1"/>
+      <c r="WG2" s="1"/>
+      <c r="WH2" s="1"/>
+      <c r="WI2" s="1"/>
+      <c r="WJ2" s="1"/>
+      <c r="WK2" s="1"/>
+      <c r="WL2" s="1"/>
+      <c r="WM2" s="1"/>
+      <c r="WN2" s="1"/>
+      <c r="WO2" s="1"/>
+      <c r="WP2" s="1"/>
+      <c r="WQ2" s="1"/>
+      <c r="WR2" s="1"/>
+      <c r="WS2" s="1"/>
+      <c r="WT2" s="1"/>
+      <c r="WU2" s="1"/>
+      <c r="WV2" s="1"/>
+      <c r="WW2" s="1"/>
+      <c r="WX2" s="1"/>
+      <c r="WY2" s="1"/>
+      <c r="WZ2" s="1"/>
+      <c r="XA2" s="1"/>
+      <c r="XB2" s="1"/>
+      <c r="XC2" s="1"/>
+      <c r="XD2" s="1"/>
+      <c r="XE2" s="1"/>
+      <c r="XF2" s="1"/>
+      <c r="XG2" s="1"/>
+      <c r="XH2" s="1"/>
+      <c r="XI2" s="1"/>
+      <c r="XJ2" s="1"/>
+      <c r="XK2" s="1"/>
+      <c r="XL2" s="1"/>
+      <c r="XM2" s="1"/>
+      <c r="XN2" s="1"/>
+      <c r="XO2" s="1"/>
+      <c r="XP2" s="1"/>
+      <c r="XQ2" s="1"/>
+      <c r="XR2" s="1"/>
+      <c r="XS2" s="1"/>
+      <c r="XT2" s="1"/>
+      <c r="XU2" s="1"/>
+      <c r="XV2" s="1"/>
+      <c r="XW2" s="1"/>
+      <c r="XX2" s="1"/>
+      <c r="XY2" s="1"/>
+      <c r="XZ2" s="1"/>
+      <c r="YA2" s="1"/>
+      <c r="YB2" s="1"/>
+      <c r="YC2" s="1"/>
+      <c r="YD2" s="1"/>
+      <c r="YE2" s="1"/>
+      <c r="YF2" s="1"/>
+      <c r="YG2" s="1"/>
+      <c r="YH2" s="1"/>
+      <c r="YI2" s="1"/>
+      <c r="YJ2" s="1"/>
+      <c r="YK2" s="1"/>
+      <c r="YL2" s="1"/>
+      <c r="YM2" s="1"/>
+      <c r="YN2" s="1"/>
+      <c r="YO2" s="1"/>
+      <c r="YP2" s="1"/>
+      <c r="YQ2" s="1"/>
+      <c r="YR2" s="1"/>
+      <c r="YS2" s="1"/>
+      <c r="YT2" s="1"/>
+      <c r="YU2" s="1"/>
+      <c r="YV2" s="1"/>
+      <c r="YW2" s="1"/>
+      <c r="YX2" s="1"/>
+      <c r="YY2" s="1"/>
+      <c r="YZ2" s="1"/>
+      <c r="ZA2" s="1"/>
+      <c r="ZB2" s="1"/>
+      <c r="ZC2" s="1"/>
+      <c r="ZD2" s="1"/>
+      <c r="ZE2" s="1"/>
+      <c r="ZF2" s="1"/>
+      <c r="ZG2" s="1"/>
+      <c r="ZH2" s="1"/>
+      <c r="ZI2" s="1"/>
+      <c r="ZJ2" s="1"/>
+      <c r="ZK2" s="1"/>
+      <c r="ZL2" s="1"/>
+      <c r="ZM2" s="1"/>
+      <c r="ZN2" s="1"/>
+      <c r="ZO2" s="1"/>
+      <c r="ZP2" s="1"/>
+      <c r="ZQ2" s="1"/>
+      <c r="ZR2" s="1"/>
+      <c r="ZS2" s="1"/>
+      <c r="ZT2" s="1"/>
+      <c r="ZU2" s="1"/>
+      <c r="ZV2" s="1"/>
+      <c r="ZW2" s="1"/>
+      <c r="ZX2" s="1"/>
+      <c r="ZY2" s="1"/>
+      <c r="ZZ2" s="1"/>
+      <c r="AAA2" s="1"/>
+      <c r="AAB2" s="1"/>
+      <c r="AAC2" s="1"/>
+      <c r="AAD2" s="1"/>
+      <c r="AAE2" s="1"/>
+      <c r="AAF2" s="1"/>
+      <c r="AAG2" s="1"/>
+      <c r="AAH2" s="1"/>
+      <c r="AAI2" s="1"/>
+      <c r="AAJ2" s="1"/>
+      <c r="AAK2" s="1"/>
+      <c r="AAL2" s="1"/>
+      <c r="AAM2" s="1"/>
+      <c r="AAN2" s="1"/>
+      <c r="AAO2" s="1"/>
+      <c r="AAP2" s="1"/>
+      <c r="AAQ2" s="1"/>
+      <c r="AAR2" s="1"/>
+      <c r="AAS2" s="1"/>
+      <c r="AAT2" s="1"/>
+      <c r="AAU2" s="1"/>
+      <c r="AAV2" s="1"/>
+      <c r="AAW2" s="1"/>
+      <c r="AAX2" s="1"/>
+      <c r="AAY2" s="1"/>
+      <c r="AAZ2" s="1"/>
+      <c r="ABA2" s="1"/>
+      <c r="ABB2" s="1"/>
+      <c r="ABC2" s="1"/>
+      <c r="ABD2" s="1"/>
+      <c r="ABE2" s="1"/>
+      <c r="ABF2" s="1"/>
+      <c r="ABG2" s="1"/>
+      <c r="ABH2" s="1"/>
+      <c r="ABI2" s="1"/>
+      <c r="ABJ2" s="1"/>
+      <c r="ABK2" s="1"/>
+      <c r="ABL2" s="1"/>
+      <c r="ABM2" s="1"/>
+      <c r="ABN2" s="1"/>
+      <c r="ABO2" s="1"/>
+      <c r="ABP2" s="1"/>
+      <c r="ABQ2" s="1"/>
+      <c r="ABR2" s="1"/>
+      <c r="ABS2" s="1"/>
+      <c r="ABT2" s="1"/>
+      <c r="ABU2" s="1"/>
+      <c r="ABV2" s="1"/>
+      <c r="ABW2" s="1"/>
+      <c r="ABX2" s="1"/>
+      <c r="ABY2" s="1"/>
+      <c r="ABZ2" s="1"/>
+      <c r="ACA2" s="1"/>
+      <c r="ACB2" s="1"/>
+      <c r="ACC2" s="1"/>
+      <c r="ACD2" s="1"/>
+      <c r="ACE2" s="1"/>
+      <c r="ACF2" s="1"/>
+      <c r="ACG2" s="1"/>
+      <c r="ACH2" s="1"/>
+      <c r="ACI2" s="1"/>
+      <c r="ACJ2" s="1"/>
+      <c r="ACK2" s="1"/>
+      <c r="ACL2" s="1"/>
+      <c r="ACM2" s="1"/>
+      <c r="ACN2" s="1"/>
+      <c r="ACO2" s="1"/>
+      <c r="ACP2" s="1"/>
+      <c r="ACQ2" s="1"/>
+      <c r="ACR2" s="1"/>
+      <c r="ACS2" s="1"/>
+      <c r="ACT2" s="1"/>
+      <c r="ACU2" s="1"/>
+      <c r="ACV2" s="1"/>
+      <c r="ACW2" s="1"/>
+      <c r="ACX2" s="1"/>
+      <c r="ACY2" s="1"/>
+      <c r="ACZ2" s="1"/>
+      <c r="ADA2" s="1"/>
+      <c r="ADB2" s="1"/>
+      <c r="ADC2" s="1"/>
+      <c r="ADD2" s="1"/>
+      <c r="ADE2" s="1"/>
+      <c r="ADF2" s="1"/>
+      <c r="ADG2" s="1"/>
+      <c r="ADH2" s="1"/>
+      <c r="ADI2" s="1"/>
+      <c r="ADJ2" s="1"/>
+      <c r="ADK2" s="1"/>
+      <c r="ADL2" s="1"/>
+      <c r="ADM2" s="1"/>
+      <c r="ADN2" s="1"/>
+      <c r="ADO2" s="1"/>
+      <c r="ADP2" s="1"/>
+      <c r="ADQ2" s="1"/>
+      <c r="ADR2" s="1"/>
+      <c r="ADS2" s="1"/>
+      <c r="ADT2" s="1"/>
+      <c r="ADU2" s="1"/>
+      <c r="ADV2" s="1"/>
+      <c r="ADW2" s="1"/>
+      <c r="ADX2" s="1"/>
+      <c r="ADY2" s="1"/>
+      <c r="ADZ2" s="1"/>
+      <c r="AEA2" s="1"/>
+      <c r="AEB2" s="1"/>
+      <c r="AEC2" s="1"/>
+      <c r="AED2" s="1"/>
+      <c r="AEE2" s="1"/>
+      <c r="AEF2" s="1"/>
+      <c r="AEG2" s="1"/>
+      <c r="AEH2" s="1"/>
+      <c r="AEI2" s="1"/>
+      <c r="AEJ2" s="1"/>
+      <c r="AEK2" s="1"/>
+      <c r="AEL2" s="1"/>
+      <c r="AEM2" s="1"/>
+      <c r="AEN2" s="1"/>
+      <c r="AEO2" s="1"/>
+      <c r="AEP2" s="1"/>
+      <c r="AEQ2" s="1"/>
+      <c r="AER2" s="1"/>
+      <c r="AES2" s="1"/>
+      <c r="AET2" s="1"/>
+      <c r="AEU2" s="1"/>
+      <c r="AEV2" s="1"/>
+      <c r="AEW2" s="1"/>
+      <c r="AEX2" s="1"/>
+      <c r="AEY2" s="1"/>
+      <c r="AEZ2" s="1"/>
+      <c r="AFA2" s="1"/>
+      <c r="AFB2" s="1"/>
+      <c r="AFC2" s="1"/>
+      <c r="AFD2" s="1"/>
+      <c r="AFE2" s="1"/>
+      <c r="AFF2" s="1"/>
+      <c r="AFG2" s="1"/>
+      <c r="AFH2" s="1"/>
+      <c r="AFI2" s="1"/>
+      <c r="AFJ2" s="1"/>
+      <c r="AFK2" s="1"/>
+      <c r="AFL2" s="1"/>
+      <c r="AFM2" s="1"/>
+      <c r="AFN2" s="1"/>
+      <c r="AFO2" s="1"/>
+      <c r="AFP2" s="1"/>
+      <c r="AFQ2" s="1"/>
+      <c r="AFR2" s="1"/>
+      <c r="AFS2" s="1"/>
+      <c r="AFT2" s="1"/>
+      <c r="AFU2" s="1"/>
+      <c r="AFV2" s="1"/>
+      <c r="AFW2" s="1"/>
+      <c r="AFX2" s="1"/>
+      <c r="AFY2" s="1"/>
+      <c r="AFZ2" s="1"/>
+      <c r="AGA2" s="1"/>
+      <c r="AGB2" s="1"/>
+      <c r="AGC2" s="1"/>
+      <c r="AGD2" s="1"/>
+      <c r="AGE2" s="1"/>
+      <c r="AGF2" s="1"/>
+      <c r="AGG2" s="1"/>
+      <c r="AGH2" s="1"/>
+      <c r="AGI2" s="1"/>
+      <c r="AGJ2" s="1"/>
+      <c r="AGK2" s="1"/>
+      <c r="AGL2" s="1"/>
+      <c r="AGM2" s="1"/>
+      <c r="AGN2" s="1"/>
+      <c r="AGO2" s="1"/>
+      <c r="AGP2" s="1"/>
+      <c r="AGQ2" s="1"/>
+      <c r="AGR2" s="1"/>
+      <c r="AGS2" s="1"/>
+      <c r="AGT2" s="1"/>
+      <c r="AGU2" s="1"/>
+      <c r="AGV2" s="1"/>
+      <c r="AGW2" s="1"/>
+      <c r="AGX2" s="1"/>
+      <c r="AGY2" s="1"/>
+      <c r="AGZ2" s="1"/>
+      <c r="AHA2" s="1"/>
+      <c r="AHB2" s="1"/>
+      <c r="AHC2" s="1"/>
+      <c r="AHD2" s="1"/>
+      <c r="AHE2" s="1"/>
+      <c r="AHF2" s="1"/>
+      <c r="AHG2" s="1"/>
+      <c r="AHH2" s="1"/>
+      <c r="AHI2" s="1"/>
+      <c r="AHJ2" s="1"/>
+      <c r="AHK2" s="1"/>
+      <c r="AHL2" s="1"/>
+      <c r="AHM2" s="1"/>
+      <c r="AHN2" s="1"/>
+      <c r="AHO2" s="1"/>
+      <c r="AHP2" s="1"/>
+      <c r="AHQ2" s="1"/>
+      <c r="AHR2" s="1"/>
+      <c r="AHS2" s="1"/>
+      <c r="AHT2" s="1"/>
+      <c r="AHU2" s="1"/>
+      <c r="AHV2" s="1"/>
+      <c r="AHW2" s="1"/>
+      <c r="AHX2" s="1"/>
+      <c r="AHY2" s="1"/>
+      <c r="AHZ2" s="1"/>
+      <c r="AIA2" s="1"/>
+      <c r="AIB2" s="1"/>
+      <c r="AIC2" s="1"/>
+      <c r="AID2" s="1"/>
+      <c r="AIE2" s="1"/>
+      <c r="AIF2" s="1"/>
+      <c r="AIG2" s="1"/>
+      <c r="AIH2" s="1"/>
+      <c r="AII2" s="1"/>
+      <c r="AIJ2" s="1"/>
+      <c r="AIK2" s="1"/>
+      <c r="AIL2" s="1"/>
+      <c r="AIM2" s="1"/>
+      <c r="AIN2" s="1"/>
+      <c r="AIO2" s="1"/>
+      <c r="AIP2" s="1"/>
+      <c r="AIQ2" s="1"/>
+      <c r="AIR2" s="1"/>
+      <c r="AIS2" s="1"/>
+      <c r="AIT2" s="1"/>
+      <c r="AIU2" s="1"/>
+      <c r="AIV2" s="1"/>
+      <c r="AIW2" s="1"/>
+      <c r="AIX2" s="1"/>
+      <c r="AIY2" s="1"/>
+      <c r="AIZ2" s="1"/>
+      <c r="AJA2" s="1"/>
+      <c r="AJB2" s="1"/>
+      <c r="AJC2" s="1"/>
+      <c r="AJD2" s="1"/>
+      <c r="AJE2" s="1"/>
+      <c r="AJF2" s="1"/>
+      <c r="AJG2" s="1"/>
+      <c r="AJH2" s="1"/>
+      <c r="AJI2" s="1"/>
+      <c r="AJJ2" s="1"/>
+      <c r="AJK2" s="1"/>
+      <c r="AJL2" s="1"/>
+      <c r="AJM2" s="1"/>
+      <c r="AJN2" s="1"/>
+      <c r="AJO2" s="1"/>
+      <c r="AJP2" s="1"/>
+      <c r="AJQ2" s="1"/>
+      <c r="AJR2" s="1"/>
+      <c r="AJS2" s="1"/>
+      <c r="AJT2" s="1"/>
+      <c r="AJU2" s="1"/>
+      <c r="AJV2" s="1"/>
+      <c r="AJW2" s="1"/>
+      <c r="AJX2" s="1"/>
+      <c r="AJY2" s="1"/>
+      <c r="AJZ2" s="1"/>
+      <c r="AKA2" s="1"/>
+      <c r="AKB2" s="1"/>
+      <c r="AKC2" s="1"/>
+      <c r="AKD2" s="1"/>
+      <c r="AKE2" s="1"/>
+      <c r="AKF2" s="1"/>
+      <c r="AKG2" s="1"/>
+      <c r="AKH2" s="1"/>
+      <c r="AKI2" s="1"/>
+      <c r="AKJ2" s="1"/>
+      <c r="AKK2" s="1"/>
+      <c r="AKL2" s="1"/>
+      <c r="AKM2" s="1"/>
+      <c r="AKN2" s="1"/>
+      <c r="AKO2" s="1"/>
+      <c r="AKP2" s="1"/>
+      <c r="AKQ2" s="1"/>
+      <c r="AKR2" s="1"/>
+      <c r="AKS2" s="1"/>
+      <c r="AKT2" s="1"/>
+      <c r="AKU2" s="1"/>
+      <c r="AKV2" s="1"/>
+      <c r="AKW2" s="1"/>
+      <c r="AKX2" s="1"/>
+      <c r="AKY2" s="1"/>
+      <c r="AKZ2" s="1"/>
+      <c r="ALA2" s="1"/>
+      <c r="ALB2" s="1"/>
+      <c r="ALC2" s="1"/>
+      <c r="ALD2" s="1"/>
+      <c r="ALE2" s="1"/>
+      <c r="ALF2" s="1"/>
+      <c r="ALG2" s="1"/>
+      <c r="ALH2" s="1"/>
+      <c r="ALI2" s="1"/>
+      <c r="ALJ2" s="1"/>
+      <c r="ALK2" s="1"/>
+      <c r="ALL2" s="1"/>
+      <c r="ALM2" s="1"/>
+      <c r="ALN2" s="1"/>
+      <c r="ALO2" s="1"/>
+      <c r="ALP2" s="1"/>
+      <c r="ALQ2" s="1"/>
+      <c r="ALR2" s="1"/>
+      <c r="ALS2" s="1"/>
+      <c r="ALT2" s="1"/>
+      <c r="ALU2" s="1"/>
+      <c r="ALV2" s="1"/>
+      <c r="ALW2" s="1"/>
+      <c r="ALX2" s="1"/>
+      <c r="ALY2" s="1"/>
+      <c r="ALZ2" s="1"/>
+      <c r="AMA2" s="1"/>
+      <c r="AMB2" s="1"/>
+      <c r="AMC2" s="1"/>
+      <c r="AMD2" s="1"/>
+      <c r="AME2" s="1"/>
+      <c r="AMF2" s="1"/>
+      <c r="AMG2" s="1"/>
+      <c r="AMH2" s="1"/>
+      <c r="AMI2" s="1"/>
+      <c r="AMJ2" s="1"/>
+      <c r="AMK2" s="1"/>
+      <c r="AML2" s="1"/>
+      <c r="AMM2" s="1"/>
+      <c r="AMN2" s="1"/>
+      <c r="AMO2" s="1"/>
+      <c r="AMP2" s="1"/>
+      <c r="AMQ2" s="1"/>
+      <c r="AMR2" s="1"/>
+      <c r="AMS2" s="1"/>
+      <c r="AMT2" s="1"/>
+      <c r="AMU2" s="1"/>
+      <c r="AMV2" s="1"/>
+      <c r="AMW2" s="1"/>
+      <c r="AMX2" s="1"/>
+      <c r="AMY2" s="1"/>
+      <c r="AMZ2" s="1"/>
+      <c r="ANA2" s="1"/>
+      <c r="ANB2" s="1"/>
+      <c r="ANC2" s="1"/>
+      <c r="AND2" s="1"/>
+      <c r="ANE2" s="1"/>
+      <c r="ANF2" s="1"/>
+      <c r="ANG2" s="1"/>
+      <c r="ANH2" s="1"/>
+      <c r="ANI2" s="1"/>
+      <c r="ANJ2" s="1"/>
+      <c r="ANK2" s="1"/>
+      <c r="ANL2" s="1"/>
+      <c r="ANM2" s="1"/>
+      <c r="ANN2" s="1"/>
+      <c r="ANO2" s="1"/>
+      <c r="ANP2" s="1"/>
+      <c r="ANQ2" s="1"/>
+      <c r="ANR2" s="1"/>
+      <c r="ANS2" s="1"/>
+      <c r="ANT2" s="1"/>
+      <c r="ANU2" s="1"/>
+      <c r="ANV2" s="1"/>
+      <c r="ANW2" s="1"/>
+      <c r="ANX2" s="1"/>
+      <c r="ANY2" s="1"/>
+      <c r="ANZ2" s="1"/>
+      <c r="AOA2" s="1"/>
+      <c r="AOB2" s="1"/>
+      <c r="AOC2" s="1"/>
+      <c r="AOD2" s="1"/>
+      <c r="AOE2" s="1"/>
+      <c r="AOF2" s="1"/>
+      <c r="AOG2" s="1"/>
+      <c r="AOH2" s="1"/>
+      <c r="AOI2" s="1"/>
+      <c r="AOJ2" s="1"/>
+      <c r="AOK2" s="1"/>
+      <c r="AOL2" s="1"/>
+      <c r="AOM2" s="1"/>
+      <c r="AON2" s="1"/>
+      <c r="AOO2" s="1"/>
+      <c r="AOP2" s="1"/>
+      <c r="AOQ2" s="1"/>
+      <c r="AOR2" s="1"/>
+      <c r="AOS2" s="1"/>
+      <c r="AOT2" s="1"/>
+      <c r="AOU2" s="1"/>
+      <c r="AOV2" s="1"/>
+      <c r="AOW2" s="1"/>
+      <c r="AOX2" s="1"/>
+      <c r="AOY2" s="1"/>
+      <c r="AOZ2" s="1"/>
+      <c r="APA2" s="1"/>
+      <c r="APB2" s="1"/>
+      <c r="APC2" s="1"/>
+      <c r="APD2" s="1"/>
+      <c r="APE2" s="1"/>
+      <c r="APF2" s="1"/>
+      <c r="APG2" s="1"/>
+      <c r="APH2" s="1"/>
+      <c r="API2" s="1"/>
+      <c r="APJ2" s="1"/>
+      <c r="APK2" s="1"/>
+      <c r="APL2" s="1"/>
+      <c r="APM2" s="1"/>
+      <c r="APN2" s="1"/>
+      <c r="APO2" s="1"/>
+      <c r="APP2" s="1"/>
+      <c r="APQ2" s="1"/>
+      <c r="APR2" s="1"/>
+      <c r="APS2" s="1"/>
+      <c r="APT2" s="1"/>
+      <c r="APU2" s="1"/>
+      <c r="APV2" s="1"/>
+      <c r="APW2" s="1"/>
+      <c r="APX2" s="1"/>
+      <c r="APY2" s="1"/>
+      <c r="APZ2" s="1"/>
+      <c r="AQA2" s="1"/>
+      <c r="AQB2" s="1"/>
+      <c r="AQC2" s="1"/>
+      <c r="AQD2" s="1"/>
+      <c r="AQE2" s="1"/>
+      <c r="AQF2" s="1"/>
+      <c r="AQG2" s="1"/>
+      <c r="AQH2" s="1"/>
+      <c r="AQI2" s="1"/>
+      <c r="AQJ2" s="1"/>
+      <c r="AQK2" s="1"/>
+      <c r="AQL2" s="1"/>
+      <c r="AQM2" s="1"/>
+      <c r="AQN2" s="1"/>
+      <c r="AQO2" s="1"/>
+      <c r="AQP2" s="1"/>
+      <c r="AQQ2" s="1"/>
+      <c r="AQR2" s="1"/>
+      <c r="AQS2" s="1"/>
+      <c r="AQT2" s="1"/>
+      <c r="AQU2" s="1"/>
+      <c r="AQV2" s="1"/>
+      <c r="AQW2" s="1"/>
+      <c r="AQX2" s="1"/>
+      <c r="AQY2" s="1"/>
+      <c r="AQZ2" s="1"/>
+      <c r="ARA2" s="1"/>
+      <c r="ARB2" s="1"/>
+      <c r="ARC2" s="1"/>
+      <c r="ARD2" s="1"/>
+      <c r="ARE2" s="1"/>
+      <c r="ARF2" s="1"/>
+      <c r="ARG2" s="1"/>
+      <c r="ARH2" s="1"/>
+      <c r="ARI2" s="1"/>
+      <c r="ARJ2" s="1"/>
+      <c r="ARK2" s="1"/>
+      <c r="ARL2" s="1"/>
+      <c r="ARM2" s="1"/>
+      <c r="ARN2" s="1"/>
+      <c r="ARO2" s="1"/>
+      <c r="ARP2" s="1"/>
+      <c r="ARQ2" s="1"/>
+      <c r="ARR2" s="1"/>
+      <c r="ARS2" s="1"/>
+      <c r="ART2" s="1"/>
+      <c r="ARU2" s="1"/>
+      <c r="ARV2" s="1"/>
+      <c r="ARW2" s="1"/>
+      <c r="ARX2" s="1"/>
+      <c r="ARY2" s="1"/>
+      <c r="ARZ2" s="1"/>
+      <c r="ASA2" s="1"/>
+      <c r="ASB2" s="1"/>
+      <c r="ASC2" s="1"/>
+      <c r="ASD2" s="1"/>
+      <c r="ASE2" s="1"/>
+      <c r="ASF2" s="1"/>
+      <c r="ASG2" s="1"/>
+      <c r="ASH2" s="1"/>
+      <c r="ASI2" s="1"/>
+      <c r="ASJ2" s="1"/>
+      <c r="ASK2" s="1"/>
+      <c r="ASL2" s="1"/>
+      <c r="ASM2" s="1"/>
+      <c r="ASN2" s="1"/>
+      <c r="ASO2" s="1"/>
+      <c r="ASP2" s="1"/>
+      <c r="ASQ2" s="1"/>
+      <c r="ASR2" s="1"/>
+      <c r="ASS2" s="1"/>
+      <c r="AST2" s="1"/>
+      <c r="ASU2" s="1"/>
+      <c r="ASV2" s="1"/>
+      <c r="ASW2" s="1"/>
+      <c r="ASX2" s="1"/>
+      <c r="ASY2" s="1"/>
+      <c r="ASZ2" s="1"/>
+      <c r="ATA2" s="1"/>
+      <c r="ATB2" s="1"/>
+      <c r="ATC2" s="1"/>
+      <c r="ATD2" s="1"/>
+      <c r="ATE2" s="1"/>
+      <c r="ATF2" s="1"/>
+      <c r="ATG2" s="1"/>
+      <c r="ATH2" s="1"/>
+      <c r="ATI2" s="1"/>
+      <c r="ATJ2" s="1"/>
+      <c r="ATK2" s="1"/>
+      <c r="ATL2" s="1"/>
+    </row>
+    <row r="3" spans="1:1208" ht="336" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="37" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1208" ht="189" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="38" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1208" ht="294" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>375</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>376</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="38" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1208" ht="189" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="38" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1208" ht="168" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>384</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>385</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="38" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1208" ht="252" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="I8" s="36" t="s">
+        <v>387</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="37" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1208" ht="168" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="38" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1208" ht="294" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="40" t="s">
+        <v>399</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="38" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>